<commit_message>
code for AccSuff w ur squared
</commit_message>
<xml_diff>
--- a/Objective values.xlsx
+++ b/Objective values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/sabetancurgi_unal_edu_co/Documents/Escritorio/S and C/accessibility-iamod_njp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CA4AC84-12D3-4F0D-81C3-B70202E6BC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{9CA4AC84-12D3-4F0D-81C3-B70202E6BC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D24B416-50F8-4BC6-9A8B-647E09066F05}"/>
   <bookViews>
     <workbookView xWindow="6192" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{24270E23-22B1-443F-A580-B5632CFE18BD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>Travel Time</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>nCar</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Utilitarian Efficiency</t>
@@ -89,7 +86,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -130,7 +127,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -147,6 +144,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,13 +467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232028DE-7396-4AB0-89C9-E207B9D70036}">
-  <dimension ref="B1:U42"/>
+  <dimension ref="B1:W48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q43" sqref="Q43"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,24 +484,24 @@
     <col min="5" max="5" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="31.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20.88671875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="31.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:23" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -511,19 +512,19 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
@@ -535,10 +536,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>2</v>
@@ -550,2487 +551,3141 @@
         <v>2</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="W3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
+      <c r="D4">
+        <v>30</v>
       </c>
       <c r="E4" s="1">
-        <v>18.555399999999999</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="F4" s="1">
-        <v>25.919499999999999</v>
+        <v>25.919489107072</v>
       </c>
       <c r="G4" s="1">
-        <v>25.919499999999999</v>
+        <v>25.919489107072</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>0.52076092736782797</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>0.52076092736782797</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>0.52076092736782797</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>0.52076092736782797</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="R4" s="1">
-        <v>0</v>
+        <v>0.52076092736782797</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>0.52076092736782797</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="U4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+        <v>25.919489107072</v>
+      </c>
+      <c r="V4" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.52076092736782797</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
       </c>
       <c r="E5" s="1">
-        <v>18.555399999999999</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="F5" s="1">
-        <v>8.0990000000000002</v>
+        <v>25.919489107072</v>
       </c>
       <c r="G5" s="1">
-        <v>8.0990000000000002</v>
+        <v>25.919489107072</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>0.57745838988499198</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>0.57745838988499198</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>0.57745838988499198</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>0.57745838988499198</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="Q5" s="1">
-        <v>0</v>
+        <v>25.919489107072</v>
       </c>
       <c r="R5" s="1">
-        <v>0</v>
+        <v>0.57745838988499198</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>0.57745838988499198</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="U5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+        <v>25.919489107072</v>
+      </c>
+      <c r="V5" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0.57745838988499198</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="G6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.62255513786699102</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.62255513786699102</v>
+      </c>
+      <c r="J6" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="K6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="L6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.62255513786699102</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.62255513786699102</v>
+      </c>
+      <c r="O6" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="P6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.62255513786699102</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0.62255513786699102</v>
+      </c>
+      <c r="T6" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="U6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="V6" s="1">
+        <v>25.919489107072</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0.62255513786699102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.29619849830543499</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.29619849830543499</v>
+      </c>
+      <c r="J7" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="K7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="L7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.29619849830543499</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.29619849830543499</v>
+      </c>
+      <c r="O7" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="P7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.29619849830543499</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.29619849830543499</v>
+      </c>
+      <c r="T7" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="U7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="V7" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.29619849830543499</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="F8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.364046965453801</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.364046965453801</v>
+      </c>
+      <c r="J8" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="L8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.364046965453801</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.364046965453801</v>
+      </c>
+      <c r="O8" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="P8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.364046965453801</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0.364046965453801</v>
+      </c>
+      <c r="T8" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="U8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="V8" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0.364046965453801</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="G9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.42208526055432499</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.42208526055432499</v>
+      </c>
+      <c r="J9" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="K9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="L9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.42208526055432499</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0.42208526055432499</v>
+      </c>
+      <c r="O9" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="P9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.42208526055432499</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0.42208526055432499</v>
+      </c>
+      <c r="T9" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="U9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="V9" s="1">
+        <v>8.0989545397086609</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.42208526055432499</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1">
-        <v>18.555399999999999</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.8172999999999999</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2.8172999999999999</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.16283968696176701</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.16283968696176701</v>
+      </c>
+      <c r="J10" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.16283968696176701</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.16283968696176701</v>
+      </c>
+      <c r="O10" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="P10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.16283968696176701</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0.16283968696176701</v>
+      </c>
+      <c r="T10" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="U10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="V10" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.16283968696176701</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>0</v>
       </c>
-      <c r="I6" s="1">
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>65</v>
+      </c>
+      <c r="E11" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.21983194134858</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.21983194134858</v>
+      </c>
+      <c r="J11" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="L11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.21983194134858</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.21983194134858</v>
+      </c>
+      <c r="O11" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="P11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.21983194134858</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0.21983194134858</v>
+      </c>
+      <c r="T11" s="1">
+        <v>18.555358915611102</v>
+      </c>
+      <c r="U11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="V11" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0.21983194134858</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B12">
         <v>0</v>
       </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0</v>
-      </c>
-      <c r="T6" s="1">
-        <v>0</v>
-      </c>
-      <c r="U6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>2000</v>
-      </c>
-      <c r="C7">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1">
-        <v>14.476900000000001</v>
-      </c>
-      <c r="F7" s="1">
-        <v>5.4537000000000004</v>
-      </c>
-      <c r="G7" s="1">
-        <v>5.4885999999999999</v>
-      </c>
-      <c r="H7" s="1">
-        <v>14.9451</v>
-      </c>
-      <c r="I7" s="1">
-        <v>3.0533999999999999</v>
-      </c>
-      <c r="J7" s="1">
-        <v>3.8197999999999999</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.50639999999999996</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0.63819999999999999</v>
-      </c>
-      <c r="M7" s="1">
-        <v>14.9308</v>
-      </c>
-      <c r="N7" s="1">
-        <v>4.2765000000000004</v>
-      </c>
-      <c r="O7" s="1">
-        <v>4.3022</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="R7" s="1">
-        <v>15.690799999999999</v>
-      </c>
-      <c r="S7" s="1">
-        <v>19.0063</v>
-      </c>
-      <c r="T7" s="1">
-        <v>19.006499999999999</v>
-      </c>
-      <c r="U7" s="1">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>2000</v>
-      </c>
-      <c r="C8">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <v>35</v>
-      </c>
-      <c r="E8" s="1">
-        <v>14.476900000000001</v>
-      </c>
-      <c r="F8" s="1">
-        <v>5.4537000000000004</v>
-      </c>
-      <c r="G8" s="1">
-        <v>5.4885999999999999</v>
-      </c>
-      <c r="H8" s="1">
-        <v>14.9451</v>
-      </c>
-      <c r="I8" s="1">
-        <v>3.0533999999999999</v>
-      </c>
-      <c r="J8" s="1">
-        <v>3.8197999999999999</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.57689999999999997</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0.68989999999999996</v>
-      </c>
-      <c r="M8" s="1">
-        <v>14.9308</v>
-      </c>
-      <c r="N8" s="1">
-        <v>4.2765000000000004</v>
-      </c>
-      <c r="O8" s="1">
-        <v>4.3022</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0.53269999999999995</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0.53269999999999995</v>
-      </c>
-      <c r="R8" s="1">
-        <v>15.679</v>
-      </c>
-      <c r="S8" s="1">
-        <v>19.5504</v>
-      </c>
-      <c r="T8" s="1">
-        <v>19.5504</v>
-      </c>
-      <c r="U8" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>2000</v>
-      </c>
-      <c r="C9">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1">
-        <v>14.476900000000001</v>
-      </c>
-      <c r="F9" s="1">
-        <v>5.4537000000000004</v>
-      </c>
-      <c r="G9" s="1">
-        <v>5.4885999999999999</v>
-      </c>
-      <c r="H9" s="1">
-        <v>14.9451</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3.0533999999999999</v>
-      </c>
-      <c r="J9" s="1">
-        <v>3.8197999999999999</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0.62980000000000003</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0.72860000000000003</v>
-      </c>
-      <c r="M9" s="1">
-        <v>14.9308</v>
-      </c>
-      <c r="N9" s="1">
-        <v>4.2765000000000004</v>
-      </c>
-      <c r="O9" s="1">
-        <v>4.3022</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0.59109999999999996</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0.59109999999999996</v>
-      </c>
-      <c r="R9" s="1">
-        <v>15.6836</v>
-      </c>
-      <c r="S9" s="1">
-        <v>19.503799999999998</v>
-      </c>
-      <c r="T9" s="1">
-        <v>19.5046</v>
-      </c>
-      <c r="U9" s="1">
-        <v>9.4000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>2000</v>
-      </c>
-      <c r="C10">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1">
-        <v>14.476900000000001</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.94740000000000002</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.95940000000000003</v>
-      </c>
-      <c r="H10" s="1">
-        <v>15.385400000000001</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.51749999999999996</v>
-      </c>
-      <c r="J10" s="1">
-        <v>6.4799999999999996E-2</v>
-      </c>
-      <c r="K10" s="1">
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0.3528</v>
-      </c>
-      <c r="M10" s="1">
-        <v>15.057399999999999</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0.44140000000000001</v>
-      </c>
-      <c r="O10" s="1">
-        <v>0.46210000000000001</v>
-      </c>
-      <c r="P10" s="1">
-        <v>6.7599999999999993E-2</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>6.7599999999999993E-2</v>
-      </c>
-      <c r="R10" s="1">
-        <v>15.550700000000001</v>
-      </c>
-      <c r="S10" s="1">
-        <v>2.5051999999999999</v>
-      </c>
-      <c r="T10" s="1">
-        <v>2.6493000000000002</v>
-      </c>
-      <c r="U10" s="1">
-        <v>2.9999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>2000</v>
-      </c>
-      <c r="C11">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1">
-        <v>14.476900000000001</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.94740000000000002</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.95940000000000003</v>
-      </c>
-      <c r="H11" s="1">
-        <v>15.385400000000001</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.51749999999999996</v>
-      </c>
-      <c r="J11" s="1">
-        <v>6.4799999999999996E-2</v>
-      </c>
-      <c r="K11" s="1">
-        <v>4.3200000000000002E-2</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0.44529999999999997</v>
-      </c>
-      <c r="M11" s="1">
-        <v>15.057399999999999</v>
-      </c>
-      <c r="N11" s="1">
-        <v>0.44140000000000001</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0.46210000000000001</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0.17560000000000001</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>0.17560000000000001</v>
-      </c>
-      <c r="R11" s="1">
-        <v>15.520899999999999</v>
-      </c>
-      <c r="S11" s="1">
-        <v>4.2328999999999999</v>
-      </c>
-      <c r="T11" s="1">
-        <v>4.2328999999999999</v>
-      </c>
-      <c r="U11" s="1">
-        <v>1.9E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>2000</v>
-      </c>
       <c r="C12">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1">
-        <v>14.476900000000001</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="F12" s="1">
-        <v>0.94740000000000002</v>
+        <v>2.81730572524503</v>
       </c>
       <c r="G12" s="1">
-        <v>0.95940000000000003</v>
+        <v>2.81730572524503</v>
       </c>
       <c r="H12" s="1">
-        <v>15.385400000000001</v>
+        <v>0.27627033627401998</v>
       </c>
       <c r="I12" s="1">
-        <v>0.51749999999999996</v>
+        <v>0.27627033627401998</v>
       </c>
       <c r="J12" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="K12" s="1">
-        <v>0.14410000000000001</v>
+        <v>2.81730572524503</v>
       </c>
       <c r="L12" s="1">
-        <v>0.51459999999999995</v>
+        <v>2.81730572524503</v>
       </c>
       <c r="M12" s="1">
-        <v>15.057399999999999</v>
+        <v>0.27627033627401998</v>
       </c>
       <c r="N12" s="1">
-        <v>0.44140000000000001</v>
+        <v>0.27627033627401998</v>
       </c>
       <c r="O12" s="1">
-        <v>0.46210000000000001</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="P12" s="1">
-        <v>0.2787</v>
+        <v>2.81730572524503</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.2787</v>
+        <v>2.81730572524503</v>
       </c>
       <c r="R12" s="1">
-        <v>15.5144</v>
+        <v>0.27627033627401998</v>
       </c>
       <c r="S12" s="1">
-        <v>4.5412999999999997</v>
+        <v>0.27627033627401998</v>
       </c>
       <c r="T12" s="1">
-        <v>4.5430999999999999</v>
+        <v>18.555358915611102</v>
       </c>
       <c r="U12" s="1">
-        <v>4.3E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="V12" s="1">
+        <v>2.81730572524503</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.27627033627401998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2000</v>
       </c>
       <c r="C13">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>30</v>
       </c>
       <c r="E13" s="1">
-        <v>14.476900000000001</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F13" s="1">
-        <v>0.1502</v>
+        <v>5.4536699274395897</v>
       </c>
       <c r="G13" s="1">
-        <v>0.15310000000000001</v>
+        <v>5.4885619342209502</v>
       </c>
       <c r="H13" s="1">
-        <v>14.533099999999999</v>
+        <v>0.18282327705947299</v>
       </c>
       <c r="I13" s="1">
-        <v>1.21E-2</v>
+        <v>0.184146089800065</v>
       </c>
       <c r="J13" s="1">
-        <v>6.8400000000000002E-2</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K13" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>3.0534292665391201</v>
       </c>
       <c r="L13" s="1">
-        <v>5.0299999999999997E-2</v>
+        <v>3.8198129450789602</v>
       </c>
       <c r="M13" s="1">
-        <v>15.267300000000001</v>
+        <v>0.28771709884039298</v>
       </c>
       <c r="N13" s="1">
-        <v>1.8599999999999998E-2</v>
+        <v>0.42482564230778402</v>
       </c>
       <c r="O13" s="1">
-        <v>1.8599999999999998E-2</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P13" s="1">
-        <v>4.3E-3</v>
+        <v>4.2765087839573201</v>
       </c>
       <c r="Q13" s="1">
-        <v>4.3E-3</v>
+        <v>4.30215675313553</v>
       </c>
       <c r="R13" s="1">
-        <v>15.4922</v>
+        <v>0.23259518537038401</v>
       </c>
       <c r="S13" s="1">
-        <v>1.1794</v>
+        <v>0.23259518537038401</v>
       </c>
       <c r="T13" s="1">
-        <v>1.1758</v>
+        <v>15.6907683421269</v>
       </c>
       <c r="U13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+        <v>19.0062674598034</v>
+      </c>
+      <c r="V13" s="1">
+        <v>19.006523481988101</v>
+      </c>
+      <c r="W13" s="1">
+        <v>6.02072767102412E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2000</v>
       </c>
       <c r="C14">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>35</v>
       </c>
       <c r="E14" s="1">
-        <v>14.476900000000001</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F14" s="1">
-        <v>0.1502</v>
+        <v>5.4536699274395897</v>
       </c>
       <c r="G14" s="1">
-        <v>0.15310000000000001</v>
+        <v>5.4885619342209502</v>
       </c>
       <c r="H14" s="1">
-        <v>14.533099999999999</v>
+        <v>0.24618092254403001</v>
       </c>
       <c r="I14" s="1">
-        <v>1.21E-2</v>
+        <v>0.247806913321797</v>
       </c>
       <c r="J14" s="1">
-        <v>6.8400000000000002E-2</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K14" s="1">
-        <v>2.1600000000000001E-2</v>
+        <v>3.0534292665391201</v>
       </c>
       <c r="L14" s="1">
-        <v>0.12189999999999999</v>
+        <v>3.8198129450789602</v>
       </c>
       <c r="M14" s="1">
-        <v>15.267300000000001</v>
+        <v>0.355796638535406</v>
       </c>
       <c r="N14" s="1">
-        <v>1.8599999999999998E-2</v>
+        <v>0.48880886535627199</v>
       </c>
       <c r="O14" s="1">
-        <v>1.8599999999999998E-2</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P14" s="1">
-        <v>5.4199999999999998E-2</v>
+        <v>4.2765087839573201</v>
       </c>
       <c r="Q14" s="1">
-        <v>5.4199999999999998E-2</v>
+        <v>4.30215675313553</v>
       </c>
       <c r="R14" s="1">
-        <v>15.365</v>
+        <v>0.30268255312697301</v>
       </c>
       <c r="S14" s="1">
-        <v>0.47989999999999999</v>
+        <v>0.30268255312697301</v>
       </c>
       <c r="T14" s="1">
-        <v>0.52239999999999998</v>
+        <v>15.6790404756375</v>
       </c>
       <c r="U14" s="1">
-        <v>6.9999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+        <v>19.550378179535301</v>
+      </c>
+      <c r="V14" s="1">
+        <v>19.5503914774281</v>
+      </c>
+      <c r="W14" s="1">
+        <v>8.2268850107369198E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2000</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D15">
         <v>40</v>
       </c>
       <c r="E15" s="1">
-        <v>14.476900000000001</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F15" s="1">
-        <v>0.1502</v>
+        <v>5.4536699274395897</v>
       </c>
       <c r="G15" s="1">
-        <v>0.15310000000000001</v>
+        <v>5.4885619342209502</v>
       </c>
       <c r="H15" s="1">
-        <v>14.533099999999999</v>
+        <v>0.30537644429959299</v>
       </c>
       <c r="I15" s="1">
-        <v>1.21E-2</v>
+        <v>0.30712216051146501</v>
       </c>
       <c r="J15" s="1">
-        <v>6.8400000000000002E-2</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K15" s="1">
-        <v>0.1174</v>
+        <v>3.0534292665391201</v>
       </c>
       <c r="L15" s="1">
-        <v>0.22189999999999999</v>
+        <v>3.8198129450789602</v>
       </c>
       <c r="M15" s="1">
-        <v>15.267300000000001</v>
+        <v>0.41422273465961901</v>
       </c>
       <c r="N15" s="1">
-        <v>1.8599999999999998E-2</v>
+        <v>0.54077415127866302</v>
       </c>
       <c r="O15" s="1">
-        <v>1.8599999999999998E-2</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P15" s="1">
-        <v>0.16259999999999999</v>
+        <v>4.2765087839573201</v>
       </c>
       <c r="Q15" s="1">
-        <v>0.16259999999999999</v>
+        <v>4.30215675313553</v>
       </c>
       <c r="R15" s="1">
-        <v>15.5131</v>
+        <v>0.36389786770483601</v>
       </c>
       <c r="S15" s="1">
-        <v>0.99419999999999997</v>
+        <v>0.36389786770483601</v>
       </c>
       <c r="T15" s="1">
-        <v>1.0019</v>
+        <v>15.6835984331488</v>
       </c>
       <c r="U15" s="1">
-        <v>3.0999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+        <v>19.503767884735499</v>
+      </c>
+      <c r="V15" s="1">
+        <v>19.504550979491398</v>
+      </c>
+      <c r="W15" s="1">
+        <v>9.4247245338952707E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B16">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>30</v>
       </c>
       <c r="E16" s="1">
-        <v>13.2742</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F16" s="1">
-        <v>3.1358000000000001</v>
+        <v>0.947396694875828</v>
       </c>
       <c r="G16" s="1">
-        <v>3.1827000000000001</v>
+        <v>0.95944694913391904</v>
       </c>
       <c r="H16" s="1">
-        <v>13.9101</v>
+        <v>3.4796354501512E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>0.77100000000000002</v>
+        <v>3.8330535514441502E-2</v>
       </c>
       <c r="J16" s="1">
-        <v>1.5173000000000001</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K16" s="1">
-        <v>0.69410000000000005</v>
+        <v>6.4820008788305405E-2</v>
       </c>
       <c r="L16" s="1">
-        <v>0.67700000000000005</v>
+        <v>0.51754399641362103</v>
       </c>
       <c r="M16" s="1">
-        <v>13.7942</v>
+        <v>4.3019402179520799E-2</v>
       </c>
       <c r="N16" s="1">
-        <v>1.8676999999999999</v>
+        <v>0.16578535371574199</v>
       </c>
       <c r="O16" s="1">
-        <v>1.8814</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P16" s="1">
-        <v>0.33439999999999998</v>
+        <v>0.44135768317820001</v>
       </c>
       <c r="Q16" s="1">
-        <v>0.33310000000000001</v>
+        <v>0.46210243513347898</v>
       </c>
       <c r="R16" s="1">
-        <v>14.5947</v>
+        <v>1.37927113841465E-2</v>
       </c>
       <c r="S16" s="1">
-        <v>15.5746</v>
+        <v>1.37927113841465E-2</v>
       </c>
       <c r="T16" s="1">
-        <v>15.5749</v>
+        <v>15.5506810100533</v>
       </c>
       <c r="U16" s="1">
-        <v>4.7999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+        <v>2.5052300847300701</v>
+      </c>
+      <c r="V16" s="1">
+        <v>2.6493334201941798</v>
+      </c>
+      <c r="W16" s="1">
+        <v>2.5898675302204099E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>35</v>
       </c>
       <c r="E17" s="1">
-        <v>13.2742</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F17" s="1">
-        <v>3.1358000000000001</v>
+        <v>0.947396694875828</v>
       </c>
       <c r="G17" s="1">
-        <v>3.1827000000000001</v>
+        <v>0.95944694913391904</v>
       </c>
       <c r="H17" s="1">
-        <v>13.9101</v>
+        <v>6.3563738517765894E-2</v>
       </c>
       <c r="I17" s="1">
-        <v>0.77100000000000002</v>
+        <v>6.94275684414776E-2</v>
       </c>
       <c r="J17" s="1">
-        <v>1.5173000000000001</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K17" s="1">
-        <v>0.73780000000000001</v>
+        <v>6.4820008788305405E-2</v>
       </c>
       <c r="L17" s="1">
-        <v>0.72309999999999997</v>
+        <v>0.51754399641362103</v>
       </c>
       <c r="M17" s="1">
-        <v>13.7942</v>
+        <v>1.4362731448747799E-2</v>
       </c>
       <c r="N17" s="1">
-        <v>1.8676999999999999</v>
+        <v>0.228608676129928</v>
       </c>
       <c r="O17" s="1">
-        <v>1.8814</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P17" s="1">
-        <v>0.42949999999999999</v>
+        <v>0.44135768317820001</v>
       </c>
       <c r="Q17" s="1">
-        <v>0.4284</v>
+        <v>0.46210243513347898</v>
       </c>
       <c r="R17" s="1">
-        <v>14.65</v>
+        <v>3.9901581891417903E-2</v>
       </c>
       <c r="S17" s="1">
-        <v>16.388500000000001</v>
+        <v>3.9901581891417903E-2</v>
       </c>
       <c r="T17" s="1">
-        <v>16.388500000000001</v>
+        <v>15.520865257280599</v>
       </c>
       <c r="U17" s="1">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+        <v>4.2328599361825896</v>
+      </c>
+      <c r="V17" s="1">
+        <v>4.2328599361825896</v>
+      </c>
+      <c r="W17" s="1">
+        <v>1.88560115810021E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B18">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C18">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D18">
         <v>40</v>
       </c>
       <c r="E18" s="1">
-        <v>13.2742</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F18" s="1">
-        <v>3.1358000000000001</v>
+        <v>0.947396694875828</v>
       </c>
       <c r="G18" s="1">
-        <v>3.1827000000000001</v>
+        <v>0.95944694913391904</v>
       </c>
       <c r="H18" s="1">
-        <v>13.9101</v>
+        <v>0.109009025198228</v>
       </c>
       <c r="I18" s="1">
-        <v>0.77100000000000002</v>
+        <v>0.116000037949139</v>
       </c>
       <c r="J18" s="1">
-        <v>1.5173000000000001</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K18" s="1">
-        <v>0.77059999999999995</v>
+        <v>6.4820008788305405E-2</v>
       </c>
       <c r="L18" s="1">
-        <v>0.75770000000000004</v>
+        <v>0.51754399641362103</v>
       </c>
       <c r="M18" s="1">
-        <v>13.7942</v>
+        <v>2.9044518804914599E-2</v>
       </c>
       <c r="N18" s="1">
-        <v>1.8676999999999999</v>
+        <v>0.28805277385884698</v>
       </c>
       <c r="O18" s="1">
-        <v>1.8814</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P18" s="1">
-        <v>0.50080000000000002</v>
+        <v>0.44135768317820001</v>
       </c>
       <c r="Q18" s="1">
-        <v>0.49980000000000002</v>
+        <v>0.46210243513347898</v>
       </c>
       <c r="R18" s="1">
-        <v>14.551399999999999</v>
+        <v>8.4590897117651304E-2</v>
       </c>
       <c r="S18" s="1">
-        <v>16.3827</v>
+        <v>8.4590897117651304E-2</v>
       </c>
       <c r="T18" s="1">
-        <v>16.3828</v>
+        <v>15.514396251254899</v>
       </c>
       <c r="U18" s="1">
-        <v>8.5000000000000006E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+        <v>4.5413212682056896</v>
+      </c>
+      <c r="V18" s="1">
+        <v>4.5430706145075703</v>
+      </c>
+      <c r="W18" s="1">
+        <v>4.3128861882991499E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C19">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>30</v>
       </c>
       <c r="E19" s="1">
-        <v>13.2742</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F19" s="1">
-        <v>0.4829</v>
+        <v>0.15019279852112</v>
       </c>
       <c r="G19" s="1">
-        <v>0.4965</v>
+        <v>0.15311860255340201</v>
       </c>
       <c r="H19" s="1">
-        <v>13.387</v>
+        <v>2.83148201061981E-2</v>
       </c>
       <c r="I19" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>2.8599463453738799E-2</v>
       </c>
       <c r="J19" s="1">
-        <v>0.20180000000000001</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K19" s="1">
-        <v>0.1038</v>
+        <v>1.2092997103909899E-2</v>
       </c>
       <c r="L19" s="1">
-        <v>0.1042</v>
+        <v>6.8396832728439105E-2</v>
       </c>
       <c r="M19" s="1">
-        <v>13.9572</v>
+        <v>5.0727452754561801E-2</v>
       </c>
       <c r="N19" s="1">
-        <v>0.1091</v>
+        <v>3.3109686406171901E-2</v>
       </c>
       <c r="O19" s="1">
-        <v>0.10929999999999999</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P19" s="1">
-        <v>2.3099999999999999E-2</v>
+        <v>1.86315859898353E-2</v>
       </c>
       <c r="Q19" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>1.8647086773335798E-2</v>
       </c>
       <c r="R19" s="1">
-        <v>14.1966</v>
+        <v>2.57765038772611E-2</v>
       </c>
       <c r="S19" s="1">
-        <v>1.4379999999999999</v>
+        <v>2.57765038772611E-2</v>
       </c>
       <c r="T19" s="1">
-        <v>1.4399</v>
+        <v>15.492172085366001</v>
       </c>
       <c r="U19" s="1">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+        <v>1.1793641690380601</v>
+      </c>
+      <c r="V19" s="1">
+        <v>1.17584155954029</v>
+      </c>
+      <c r="W19" s="1">
+        <v>9.4054337214562895E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D20">
         <v>35</v>
       </c>
       <c r="E20" s="1">
-        <v>13.2742</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F20" s="1">
-        <v>0.4829</v>
+        <v>0.15019279852112</v>
       </c>
       <c r="G20" s="1">
-        <v>0.4965</v>
+        <v>0.15311860255340201</v>
       </c>
       <c r="H20" s="1">
-        <v>13.387</v>
+        <v>2.3152309713084501E-2</v>
       </c>
       <c r="I20" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>2.4243859984168E-2</v>
       </c>
       <c r="J20" s="1">
-        <v>0.20180000000000001</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K20" s="1">
-        <v>0.17899999999999999</v>
+        <v>1.2092997103909899E-2</v>
       </c>
       <c r="L20" s="1">
-        <v>0.18429999999999999</v>
+        <v>6.8396832728439105E-2</v>
       </c>
       <c r="M20" s="1">
-        <v>13.9572</v>
+        <v>1.09105606668698E-2</v>
       </c>
       <c r="N20" s="1">
-        <v>0.1091</v>
+        <v>3.4018741863485899E-2</v>
       </c>
       <c r="O20" s="1">
-        <v>0.10929999999999999</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P20" s="1">
-        <v>9.4700000000000006E-2</v>
+        <v>1.86315859898353E-2</v>
       </c>
       <c r="Q20" s="1">
-        <v>9.3700000000000006E-2</v>
+        <v>1.8647086773335798E-2</v>
       </c>
       <c r="R20" s="1">
-        <v>14.292</v>
+        <v>9.2562442506826294E-3</v>
       </c>
       <c r="S20" s="1">
-        <v>2.3344999999999998</v>
+        <v>9.2562442506826294E-3</v>
       </c>
       <c r="T20" s="1">
-        <v>2.2452999999999999</v>
+        <v>15.364969014623099</v>
       </c>
       <c r="U20" s="1">
-        <v>1.1999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.47987204632595798</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0.52240024224002202</v>
+      </c>
+      <c r="W20" s="1">
+        <v>6.5393883819689499E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D21">
         <v>40</v>
       </c>
       <c r="E21" s="1">
-        <v>13.2742</v>
+        <v>14.476947683902701</v>
       </c>
       <c r="F21" s="1">
-        <v>0.4829</v>
+        <v>0.15019279852112</v>
       </c>
       <c r="G21" s="1">
-        <v>0.4965</v>
+        <v>0.15311860255340201</v>
       </c>
       <c r="H21" s="1">
-        <v>13.387</v>
+        <v>5.0774887938424197E-2</v>
       </c>
       <c r="I21" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>5.2286212408029102E-2</v>
       </c>
       <c r="J21" s="1">
-        <v>0.20180000000000001</v>
+        <v>14.533115604981001</v>
       </c>
       <c r="K21" s="1">
-        <v>0.2757</v>
+        <v>1.2092997103909899E-2</v>
       </c>
       <c r="L21" s="1">
-        <v>0.28149999999999997</v>
+        <v>6.8396832728439105E-2</v>
       </c>
       <c r="M21" s="1">
-        <v>13.9572</v>
+        <v>1.9422603846703301E-2</v>
       </c>
       <c r="N21" s="1">
-        <v>0.1091</v>
+        <v>6.4716999874991105E-2</v>
       </c>
       <c r="O21" s="1">
-        <v>0.10929999999999999</v>
+        <v>15.2672628683067</v>
       </c>
       <c r="P21" s="1">
-        <v>0.1991</v>
+        <v>1.86315859898353E-2</v>
       </c>
       <c r="Q21" s="1">
-        <v>0.1983</v>
+        <v>1.8647086773335798E-2</v>
       </c>
       <c r="R21" s="1">
-        <v>14.344900000000001</v>
+        <v>3.0924340577898401E-2</v>
       </c>
       <c r="S21" s="1">
-        <v>3.0188000000000001</v>
+        <v>3.0924340577898401E-2</v>
       </c>
       <c r="T21" s="1">
-        <v>3.0202</v>
+        <v>15.513054290946</v>
       </c>
       <c r="U21" s="1">
-        <v>3.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.99416038552628705</v>
+      </c>
+      <c r="V21" s="1">
+        <v>1.0019474124377501</v>
+      </c>
+      <c r="W21" s="1">
+        <v>3.0622499821415699E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>3000</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>30</v>
       </c>
       <c r="E22" s="1">
-        <v>13.2742</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F22" s="1">
-        <v>6.5000000000000002E-2</v>
+        <v>3.1358436516625599</v>
       </c>
       <c r="G22" s="1">
-        <v>6.5199999999999994E-2</v>
+        <v>3.1927102218673</v>
       </c>
       <c r="H22" s="1">
-        <v>13.290699999999999</v>
+        <v>0.118877022961958</v>
       </c>
       <c r="I22" s="1">
-        <v>1.21E-2</v>
+        <v>0.121167345286568</v>
       </c>
       <c r="J22" s="1">
-        <v>2.87E-2</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K22" s="1">
-        <v>8.6E-3</v>
+        <v>0.95660881850706503</v>
       </c>
       <c r="L22" s="1">
-        <v>1.4E-2</v>
+        <v>1.52829008711982</v>
       </c>
       <c r="M22" s="1">
-        <v>14.510199999999999</v>
+        <v>0.18274180298592799</v>
       </c>
       <c r="N22" s="1">
-        <v>1.21E-2</v>
+        <v>0.39082204284432998</v>
       </c>
       <c r="O22" s="1">
-        <v>1.21E-2</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P22" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>1.86771857812426</v>
       </c>
       <c r="Q22" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>1.8813854888972199</v>
       </c>
       <c r="R22" s="1">
-        <v>14.2662</v>
+        <v>0.14245997729996601</v>
       </c>
       <c r="S22" s="1">
-        <v>0.51529999999999998</v>
+        <v>0.141902794644062</v>
       </c>
       <c r="T22" s="1">
-        <v>0.60170000000000001</v>
+        <v>14.5947445747959</v>
       </c>
       <c r="U22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+        <v>15.574646849745999</v>
+      </c>
+      <c r="V22" s="1">
+        <v>15.5748949626495</v>
+      </c>
+      <c r="W22" s="1">
+        <v>4.8070695525870904E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>3000</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D23">
         <v>35</v>
       </c>
       <c r="E23" s="1">
-        <v>13.2742</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F23" s="1">
-        <v>6.5000000000000002E-2</v>
+        <v>3.1358436516625599</v>
       </c>
       <c r="G23" s="1">
-        <v>6.5199999999999994E-2</v>
+        <v>3.1927102218673</v>
       </c>
       <c r="H23" s="1">
-        <v>13.290699999999999</v>
+        <v>0.17165065726269099</v>
       </c>
       <c r="I23" s="1">
-        <v>1.21E-2</v>
+        <v>0.175804073468805</v>
       </c>
       <c r="J23" s="1">
-        <v>2.87E-2</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K23" s="1">
-        <v>4.5499999999999999E-2</v>
+        <v>0.95660881850706503</v>
       </c>
       <c r="L23" s="1">
-        <v>5.2400000000000002E-2</v>
+        <v>1.52829008711982</v>
       </c>
       <c r="M23" s="1">
-        <v>14.510199999999999</v>
+        <v>0.24180180508520299</v>
       </c>
       <c r="N23" s="1">
-        <v>1.21E-2</v>
+        <v>0.457413780284598</v>
       </c>
       <c r="O23" s="1">
-        <v>1.21E-2</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P23" s="1">
-        <v>2.1600000000000001E-2</v>
+        <v>1.86771857812426</v>
       </c>
       <c r="Q23" s="1">
-        <v>2.1600000000000001E-2</v>
+        <v>1.8813854888972199</v>
       </c>
       <c r="R23" s="1">
-        <v>14.1836</v>
+        <v>0.20696565789684701</v>
       </c>
       <c r="S23" s="1">
-        <v>0.13769999999999999</v>
+        <v>0.20624140791397599</v>
       </c>
       <c r="T23" s="1">
-        <v>0.13769999999999999</v>
+        <v>14.559977366042</v>
       </c>
       <c r="U23" s="1">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+        <v>16.388541675938502</v>
+      </c>
+      <c r="V23" s="1">
+        <v>16.388541675938502</v>
+      </c>
+      <c r="W23" s="1">
+        <v>7.0038676231975704E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>3000</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <v>40</v>
       </c>
       <c r="E24" s="1">
-        <v>13.2742</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F24" s="1">
-        <v>6.5000000000000002E-2</v>
+        <v>3.1358436516625599</v>
       </c>
       <c r="G24" s="1">
-        <v>6.5199999999999994E-2</v>
+        <v>3.1927102218673</v>
       </c>
       <c r="H24" s="1">
-        <v>13.290699999999999</v>
+        <v>0.22722174351739399</v>
       </c>
       <c r="I24" s="1">
-        <v>1.21E-2</v>
+        <v>0.23229335577541299</v>
       </c>
       <c r="J24" s="1">
-        <v>2.87E-2</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K24" s="1">
-        <v>0.14649999999999999</v>
+        <v>0.95660881850706503</v>
       </c>
       <c r="L24" s="1">
-        <v>0.15429999999999999</v>
+        <v>1.52829008711982</v>
       </c>
       <c r="M24" s="1">
-        <v>14.510199999999999</v>
+        <v>0.29871674985713298</v>
       </c>
       <c r="N24" s="1">
-        <v>1.21E-2</v>
+        <v>0.511827451960854</v>
       </c>
       <c r="O24" s="1">
-        <v>1.21E-2</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P24" s="1">
-        <v>0.1203</v>
+        <v>1.86771857812426</v>
       </c>
       <c r="Q24" s="1">
-        <v>0.1203</v>
+        <v>1.8813854888972199</v>
       </c>
       <c r="R24" s="1">
-        <v>14.0868</v>
+        <v>0.26803242642331598</v>
       </c>
       <c r="S24" s="1">
-        <v>9.5799999999999996E-2</v>
+        <v>0.26723683388099201</v>
       </c>
       <c r="T24" s="1">
-        <v>9.5799999999999996E-2</v>
+        <v>14.551429352652701</v>
       </c>
       <c r="U24" s="1">
-        <v>2.8999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+        <v>16.382721600328999</v>
+      </c>
+      <c r="V24" s="1">
+        <v>16.382772260880099</v>
+      </c>
+      <c r="W24" s="1">
+        <v>8.4878830630759298E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B25">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C25">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D25">
         <v>30</v>
       </c>
       <c r="E25" s="1">
-        <v>12.3377</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F25" s="1">
-        <v>1.4728000000000001</v>
+        <v>0.48292223095732401</v>
       </c>
       <c r="G25" s="1">
-        <v>1.5162</v>
+        <v>0.49646393678310102</v>
       </c>
       <c r="H25" s="1">
-        <v>13.3711</v>
+        <v>2.7254188791262901E-2</v>
       </c>
       <c r="I25" s="1">
-        <v>0.41120000000000001</v>
+        <v>2.6659602670032E-2</v>
       </c>
       <c r="J25" s="1">
-        <v>0.74670000000000003</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K25" s="1">
-        <v>0.56040000000000001</v>
+        <v>6.481992658164E-2</v>
       </c>
       <c r="L25" s="1">
-        <v>0.40539999999999998</v>
+        <v>0.20174985452442301</v>
       </c>
       <c r="M25" s="1">
-        <v>12.765499999999999</v>
+        <v>4.4681901881880502E-2</v>
       </c>
       <c r="N25" s="1">
-        <v>0.7097</v>
+        <v>4.3636053368891398E-2</v>
       </c>
       <c r="O25" s="1">
-        <v>0.71240000000000003</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P25" s="1">
-        <v>0.2354</v>
+        <v>0.109058763220056</v>
       </c>
       <c r="Q25" s="1">
-        <v>0.2354</v>
+        <v>0.109303819080486</v>
       </c>
       <c r="R25" s="1">
-        <v>13.445499999999999</v>
+        <v>1.9229706883824998E-2</v>
       </c>
       <c r="S25" s="1">
-        <v>10.6526</v>
+        <v>1.89696883110698E-2</v>
       </c>
       <c r="T25" s="1">
-        <v>10.6439</v>
+        <v>14.1965967559644</v>
       </c>
       <c r="U25" s="1">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+        <v>1.43796441332221</v>
+      </c>
+      <c r="V25" s="1">
+        <v>1.43992870549402</v>
+      </c>
+      <c r="W25" s="1">
+        <v>2.09697518076688E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B26">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D26">
         <v>35</v>
       </c>
       <c r="E26" s="1">
-        <v>12.3377</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F26" s="1">
-        <v>1.4728000000000001</v>
+        <v>0.48292223095732401</v>
       </c>
       <c r="G26" s="1">
-        <v>1.5162</v>
+        <v>0.49646393678310102</v>
       </c>
       <c r="H26" s="1">
-        <v>13.3711</v>
+        <v>2.7031712177691999E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>0.41120000000000001</v>
+        <v>2.90438821431852E-2</v>
       </c>
       <c r="J26" s="1">
-        <v>0.74670000000000003</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K26" s="1">
-        <v>0.62319999999999998</v>
+        <v>6.481992658164E-2</v>
       </c>
       <c r="L26" s="1">
-        <v>0.4904</v>
+        <v>0.20174985452442301</v>
       </c>
       <c r="M26" s="1">
-        <v>12.765499999999999</v>
+        <v>1.34219062294537E-2</v>
       </c>
       <c r="N26" s="1">
-        <v>0.7097</v>
+        <v>6.2741799341352406E-2</v>
       </c>
       <c r="O26" s="1">
-        <v>0.71240000000000003</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P26" s="1">
-        <v>0.34460000000000002</v>
+        <v>0.109058763220056</v>
       </c>
       <c r="Q26" s="1">
-        <v>0.34460000000000002</v>
+        <v>0.109303819080486</v>
       </c>
       <c r="R26" s="1">
-        <v>13.507</v>
+        <v>1.7913641061825102E-2</v>
       </c>
       <c r="S26" s="1">
-        <v>11.986599999999999</v>
+        <v>1.7449701217725499E-2</v>
       </c>
       <c r="T26" s="1">
-        <v>11.9925</v>
+        <v>14.2919997464018</v>
       </c>
       <c r="U26" s="1">
-        <v>6.6E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+        <v>2.33446481434741</v>
+      </c>
+      <c r="V26" s="1">
+        <v>2.2453330552775101</v>
+      </c>
+      <c r="W26" s="1">
+        <v>1.15852298487793E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B27">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C27">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D27">
         <v>40</v>
       </c>
       <c r="E27" s="1">
-        <v>12.3377</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F27" s="1">
-        <v>1.4728000000000001</v>
+        <v>0.48292223095732401</v>
       </c>
       <c r="G27" s="1">
-        <v>1.5162</v>
+        <v>0.49646393678310102</v>
       </c>
       <c r="H27" s="1">
-        <v>13.3711</v>
+        <v>5.7311828077005501E-2</v>
       </c>
       <c r="I27" s="1">
-        <v>0.41120000000000001</v>
+        <v>6.0727418029859301E-2</v>
       </c>
       <c r="J27" s="1">
-        <v>0.74670000000000003</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K27" s="1">
-        <v>0.67030000000000001</v>
+        <v>6.481992658164E-2</v>
       </c>
       <c r="L27" s="1">
-        <v>0.55410000000000004</v>
+        <v>0.20174985452442301</v>
       </c>
       <c r="M27" s="1">
-        <v>12.765499999999999</v>
+        <v>2.6668724105293199E-2</v>
       </c>
       <c r="N27" s="1">
-        <v>0.7097</v>
+        <v>0.102778100221444</v>
       </c>
       <c r="O27" s="1">
-        <v>0.71240000000000003</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P27" s="1">
-        <v>0.42649999999999999</v>
+        <v>0.109058763220056</v>
       </c>
       <c r="Q27" s="1">
-        <v>0.42649999999999999</v>
+        <v>0.109303819080486</v>
       </c>
       <c r="R27" s="1">
-        <v>13.5069</v>
+        <v>4.78635527537681E-2</v>
       </c>
       <c r="S27" s="1">
-        <v>11.9712</v>
+        <v>4.7299405314665303E-2</v>
       </c>
       <c r="T27" s="1">
-        <v>11.9709</v>
+        <v>14.3449073829388</v>
       </c>
       <c r="U27" s="1">
-        <v>8.0999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+        <v>3.0187565911988199</v>
+      </c>
+      <c r="V27" s="1">
+        <v>3.0202021979013201</v>
+      </c>
+      <c r="W27" s="1">
+        <v>3.5851891206514701E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C28">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D28">
         <v>30</v>
       </c>
       <c r="E28" s="1">
-        <v>12.3377</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F28" s="1">
-        <v>0.20019999999999999</v>
+        <v>6.4969801329223406E-2</v>
       </c>
       <c r="G28" s="1">
-        <v>0.20369999999999999</v>
+        <v>6.5218522247180805E-2</v>
       </c>
       <c r="H28" s="1">
-        <v>12.369199999999999</v>
+        <v>4.0497991920057798E-2</v>
       </c>
       <c r="I28" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>3.8607003674865699E-2</v>
       </c>
       <c r="J28" s="1">
-        <v>0.1125</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K28" s="1">
-        <v>3.1199999999999999E-2</v>
+        <v>1.2092997092051701E-2</v>
       </c>
       <c r="L28" s="1">
-        <v>3.7600000000000001E-2</v>
+        <v>2.8706445963321801E-2</v>
       </c>
       <c r="M28" s="1">
-        <v>13.0791</v>
+        <v>5.0727452754561801E-2</v>
       </c>
       <c r="N28" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>3.8291524791453403E-2</v>
       </c>
       <c r="O28" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P28" s="1">
-        <v>6.3E-3</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="Q28" s="1">
-        <v>6.3E-3</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="R28" s="1">
-        <v>13.1732</v>
+        <v>4.90166757943028E-2</v>
       </c>
       <c r="S28" s="1">
-        <v>0.98180000000000001</v>
+        <v>4.90166757943028E-2</v>
       </c>
       <c r="T28" s="1">
-        <v>0.98670000000000002</v>
+        <v>14.266180131436499</v>
       </c>
       <c r="U28" s="1">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.51353306983106295</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0.601716995400984</v>
+      </c>
+      <c r="W28" s="1">
+        <v>9.4054337214562895E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B29">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C29">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D29">
         <v>35</v>
       </c>
       <c r="E29" s="1">
-        <v>12.3377</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F29" s="1">
-        <v>0.20019999999999999</v>
+        <v>6.4969801329223406E-2</v>
       </c>
       <c r="G29" s="1">
-        <v>0.20369999999999999</v>
+        <v>6.5218522247180805E-2</v>
       </c>
       <c r="H29" s="1">
-        <v>12.369199999999999</v>
+        <v>1.37555452211601E-2</v>
       </c>
       <c r="I29" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>1.3502043148854699E-2</v>
       </c>
       <c r="J29" s="1">
-        <v>0.1125</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K29" s="1">
-        <v>7.4499999999999997E-2</v>
+        <v>1.2092997092051701E-2</v>
       </c>
       <c r="L29" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>2.8706445963321801E-2</v>
       </c>
       <c r="M29" s="1">
-        <v>13.0791</v>
+        <v>1.09105606668698E-2</v>
       </c>
       <c r="N29" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>1.49681974368432E-2</v>
       </c>
       <c r="O29" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P29" s="1">
-        <v>4.0099999999999997E-2</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="Q29" s="1">
-        <v>4.0099999999999997E-2</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="R29" s="1">
-        <v>13.0244</v>
+        <v>1.05958588878797E-2</v>
       </c>
       <c r="S29" s="1">
-        <v>0.89449999999999996</v>
+        <v>1.05958588878797E-2</v>
       </c>
       <c r="T29" s="1">
-        <v>0.89449999999999996</v>
+        <v>14.183587898088399</v>
       </c>
       <c r="U29" s="1">
-        <v>1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.13768856848139599</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0.13768856848139599</v>
+      </c>
+      <c r="W29" s="1">
+        <v>6.1772633905336999E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B30">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C30">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D30">
         <v>40</v>
       </c>
       <c r="E30" s="1">
-        <v>12.3377</v>
+        <v>13.274226568124901</v>
       </c>
       <c r="F30" s="1">
-        <v>0.20019999999999999</v>
+        <v>6.4969801329223406E-2</v>
       </c>
       <c r="G30" s="1">
-        <v>0.20369999999999999</v>
+        <v>6.5218522247180805E-2</v>
       </c>
       <c r="H30" s="1">
-        <v>12.369199999999999</v>
+        <v>2.9533058164868901E-2</v>
       </c>
       <c r="I30" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>3.0208564004571802E-2</v>
       </c>
       <c r="J30" s="1">
-        <v>0.1125</v>
+        <v>13.290702563725</v>
       </c>
       <c r="K30" s="1">
-        <v>0.17649999999999999</v>
+        <v>1.2092997092051701E-2</v>
       </c>
       <c r="L30" s="1">
-        <v>0.18390000000000001</v>
+        <v>2.8706445963321801E-2</v>
       </c>
       <c r="M30" s="1">
-        <v>13.0791</v>
+        <v>1.9422603846703301E-2</v>
       </c>
       <c r="N30" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>3.26310696299736E-2</v>
       </c>
       <c r="O30" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>14.510210140560201</v>
       </c>
       <c r="P30" s="1">
-        <v>0.13950000000000001</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="Q30" s="1">
-        <v>0.13950000000000001</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="R30" s="1">
-        <v>12.970499999999999</v>
+        <v>1.9903028787770598E-2</v>
       </c>
       <c r="S30" s="1">
-        <v>0.74690000000000001</v>
+        <v>1.9903028787770598E-2</v>
       </c>
       <c r="T30" s="1">
-        <v>0.753</v>
+        <v>14.086816463182201</v>
       </c>
       <c r="U30" s="1">
-        <v>3.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+        <v>9.5840796137552503E-2</v>
+      </c>
+      <c r="V30" s="1">
+        <v>9.5840796137552503E-2</v>
+      </c>
+      <c r="W30" s="1">
+        <v>2.9346180977212499E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>4000</v>
       </c>
       <c r="C31">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D31">
         <v>30</v>
       </c>
       <c r="E31" s="1">
-        <v>12.3377</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F31" s="1">
-        <v>2.2599999999999999E-2</v>
+        <v>1.4728077275612399</v>
       </c>
       <c r="G31" s="1">
-        <v>2.2599999999999999E-2</v>
+        <v>1.5161796149334901</v>
       </c>
       <c r="H31" s="1">
-        <v>12.3466</v>
+        <v>9.2781726472525805E-2</v>
       </c>
       <c r="I31" s="1">
-        <v>1.21E-2</v>
+        <v>9.8380102547007298E-2</v>
       </c>
       <c r="J31" s="1">
-        <v>1.7600000000000001E-2</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K31" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.41113750540480898</v>
       </c>
       <c r="L31" s="1">
-        <v>3.5999999999999999E-3</v>
+        <v>0.73697440663198899</v>
       </c>
       <c r="M31" s="1">
-        <v>14.443300000000001</v>
+        <v>4.82993428102007E-2</v>
       </c>
       <c r="N31" s="1">
-        <v>1.21E-2</v>
+        <v>0.20106553245866801</v>
       </c>
       <c r="O31" s="1">
-        <v>1.21E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P31" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.70967292668672799</v>
       </c>
       <c r="Q31" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.71239118513739597</v>
       </c>
       <c r="R31" s="1">
-        <v>13.382899999999999</v>
+        <v>8.8391809732441207E-2</v>
       </c>
       <c r="S31" s="1">
-        <v>0.50509999999999999</v>
+        <v>8.8391809732441207E-2</v>
       </c>
       <c r="T31" s="1">
-        <v>0.5454</v>
+        <v>13.4455091631944</v>
       </c>
       <c r="U31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+        <v>10.6526413833353</v>
+      </c>
+      <c r="V31" s="1">
+        <v>10.6438539044631</v>
+      </c>
+      <c r="W31" s="1">
+        <v>4.4934757244565098E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>4000</v>
       </c>
       <c r="C32">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D32">
         <v>35</v>
       </c>
       <c r="E32" s="1">
-        <v>12.3377</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F32" s="1">
-        <v>2.2599999999999999E-2</v>
+        <v>1.4728077275612399</v>
       </c>
       <c r="G32" s="1">
-        <v>2.2599999999999999E-2</v>
+        <v>1.5161796149334901</v>
       </c>
       <c r="H32" s="1">
-        <v>12.3466</v>
+        <v>0.135622733985372</v>
       </c>
       <c r="I32" s="1">
-        <v>1.21E-2</v>
+        <v>0.141065076076863</v>
       </c>
       <c r="J32" s="1">
-        <v>1.7600000000000001E-2</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K32" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>0.41113750540480898</v>
       </c>
       <c r="L32" s="1">
-        <v>3.3700000000000001E-2</v>
+        <v>0.73697440663198899</v>
       </c>
       <c r="M32" s="1">
-        <v>14.443300000000001</v>
+        <v>8.0502586919473901E-2</v>
       </c>
       <c r="N32" s="1">
-        <v>1.21E-2</v>
+        <v>0.26762770227027899</v>
       </c>
       <c r="O32" s="1">
-        <v>1.21E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P32" s="1">
-        <v>2.1600000000000001E-2</v>
+        <v>0.70967292668672799</v>
       </c>
       <c r="Q32" s="1">
-        <v>2.1600000000000001E-2</v>
+        <v>0.71239118513739597</v>
       </c>
       <c r="R32" s="1">
-        <v>13.076499999999999</v>
+        <v>0.14298658358979</v>
       </c>
       <c r="S32" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>0.14298658358979</v>
       </c>
       <c r="T32" s="1">
-        <v>3.4500000000000003E-2</v>
+        <v>13.507023206513299</v>
       </c>
       <c r="U32" s="1">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+        <v>11.986642717232399</v>
+      </c>
+      <c r="V32" s="1">
+        <v>11.992529156781099</v>
+      </c>
+      <c r="W32" s="1">
+        <v>6.5698424523034397E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>4000</v>
       </c>
       <c r="C33">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D33">
         <v>40</v>
       </c>
       <c r="E33" s="1">
-        <v>12.3377</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F33" s="1">
-        <v>2.2599999999999999E-2</v>
+        <v>1.4728077275612399</v>
       </c>
       <c r="G33" s="1">
-        <v>2.2599999999999999E-2</v>
+        <v>1.5161796149334901</v>
       </c>
       <c r="H33" s="1">
-        <v>12.3466</v>
+        <v>0.186732590274305</v>
       </c>
       <c r="I33" s="1">
-        <v>1.21E-2</v>
+        <v>0.19191709006000399</v>
       </c>
       <c r="J33" s="1">
-        <v>1.7600000000000001E-2</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K33" s="1">
-        <v>0.12230000000000001</v>
+        <v>0.41113750540480898</v>
       </c>
       <c r="L33" s="1">
-        <v>0.13100000000000001</v>
+        <v>0.73697440663198899</v>
       </c>
       <c r="M33" s="1">
-        <v>14.443300000000001</v>
+        <v>0.127351205889706</v>
       </c>
       <c r="N33" s="1">
-        <v>1.21E-2</v>
+        <v>0.32795555709336399</v>
       </c>
       <c r="O33" s="1">
-        <v>1.21E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P33" s="1">
-        <v>0.1203</v>
+        <v>0.70967292668672799</v>
       </c>
       <c r="Q33" s="1">
-        <v>0.1203</v>
+        <v>0.71239118513739597</v>
       </c>
       <c r="R33" s="1">
-        <v>13.08</v>
+        <v>0.20047781314736801</v>
       </c>
       <c r="S33" s="1">
-        <v>8.8999999999999996E-2</v>
+        <v>0.20047781314736801</v>
       </c>
       <c r="T33" s="1">
-        <v>8.8999999999999996E-2</v>
+        <v>13.506936703965399</v>
       </c>
       <c r="U33" s="1">
-        <v>2.8999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+        <v>11.9711502929815</v>
+      </c>
+      <c r="V33" s="1">
+        <v>11.970911727915301</v>
+      </c>
+      <c r="W33" s="1">
+        <v>8.1496446174726695E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B34">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C34">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D34">
         <v>30</v>
       </c>
       <c r="E34" s="1">
-        <v>11.6381</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F34" s="1">
-        <v>0.75280000000000002</v>
+        <v>0.20017590725284001</v>
       </c>
       <c r="G34" s="1">
-        <v>0.749</v>
+        <v>0.20369666675711001</v>
       </c>
       <c r="H34" s="1">
-        <v>11.713699999999999</v>
+        <v>3.2404854314990697E-2</v>
       </c>
       <c r="I34" s="1">
-        <v>0.41110000000000002</v>
+        <v>3.3597876038764699E-2</v>
       </c>
       <c r="J34" s="1">
-        <v>0.45069999999999999</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K34" s="1">
-        <v>0.1797</v>
+        <v>6.48199265529356E-2</v>
       </c>
       <c r="L34" s="1">
-        <v>0.18629999999999999</v>
+        <v>0.112542641760282</v>
       </c>
       <c r="M34" s="1">
-        <v>11.970599999999999</v>
+        <v>4.4681901881880502E-2</v>
       </c>
       <c r="N34" s="1">
-        <v>0.4118</v>
+        <v>3.2626655872244802E-2</v>
       </c>
       <c r="O34" s="1">
-        <v>0.4118</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P34" s="1">
-        <v>0.14510000000000001</v>
+        <v>6.4820172017016203E-2</v>
       </c>
       <c r="Q34" s="1">
-        <v>0.14510000000000001</v>
+        <v>6.4821297126004901E-2</v>
       </c>
       <c r="R34" s="1">
-        <v>12.599299999999999</v>
+        <v>4.2041693454294399E-2</v>
       </c>
       <c r="S34" s="1">
-        <v>6.4513999999999996</v>
+        <v>4.2041693454294399E-2</v>
       </c>
       <c r="T34" s="1">
-        <v>6.5858999999999996</v>
+        <v>13.173204705537501</v>
       </c>
       <c r="U34" s="1">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.98175480704001195</v>
+      </c>
+      <c r="V34" s="1">
+        <v>0.98668828456444402</v>
+      </c>
+      <c r="W34" s="1">
+        <v>2.09697518076688E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B35">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C35">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D35">
         <v>35</v>
       </c>
       <c r="E35" s="1">
-        <v>11.6381</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F35" s="1">
-        <v>0.75280000000000002</v>
+        <v>0.20017590725284001</v>
       </c>
       <c r="G35" s="1">
-        <v>0.749</v>
+        <v>0.20369666675711001</v>
       </c>
       <c r="H35" s="1">
-        <v>11.713699999999999</v>
+        <v>1.76194509520359E-2</v>
       </c>
       <c r="I35" s="1">
-        <v>0.41110000000000002</v>
+        <v>2.0054085495902801E-2</v>
       </c>
       <c r="J35" s="1">
-        <v>0.45069999999999999</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K35" s="1">
-        <v>0.27989999999999998</v>
+        <v>6.48199265529356E-2</v>
       </c>
       <c r="L35" s="1">
-        <v>0.28549999999999998</v>
+        <v>0.112542641760282</v>
       </c>
       <c r="M35" s="1">
-        <v>11.970599999999999</v>
+        <v>1.34219062294537E-2</v>
       </c>
       <c r="N35" s="1">
-        <v>0.4118</v>
+        <v>2.2790636648973499E-2</v>
       </c>
       <c r="O35" s="1">
-        <v>0.4118</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P35" s="1">
-        <v>0.25009999999999999</v>
+        <v>6.4820172017016203E-2</v>
       </c>
       <c r="Q35" s="1">
-        <v>0.24940000000000001</v>
+        <v>6.4821297126004901E-2</v>
       </c>
       <c r="R35" s="1">
-        <v>12.804399999999999</v>
+        <v>1.25167832687758E-2</v>
       </c>
       <c r="S35" s="1">
-        <v>8.9799000000000007</v>
+        <v>1.25167832687758E-2</v>
       </c>
       <c r="T35" s="1">
-        <v>9.0038</v>
+        <v>13.024396645161399</v>
       </c>
       <c r="U35" s="1">
-        <v>6.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.894494668949945</v>
+      </c>
+      <c r="V35" s="1">
+        <v>0.894494668949946</v>
+      </c>
+      <c r="W35" s="1">
+        <v>1.1223104857344E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B36">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C36">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D36">
         <v>40</v>
       </c>
       <c r="E36" s="1">
-        <v>11.6381</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F36" s="1">
-        <v>0.75280000000000002</v>
+        <v>0.20017590725284001</v>
       </c>
       <c r="G36" s="1">
-        <v>0.749</v>
+        <v>0.20369666675711001</v>
       </c>
       <c r="H36" s="1">
-        <v>11.713699999999999</v>
+        <v>4.0002053718122703E-2</v>
       </c>
       <c r="I36" s="1">
-        <v>0.41110000000000002</v>
+        <v>4.3059013143796003E-2</v>
       </c>
       <c r="J36" s="1">
-        <v>0.45069999999999999</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K36" s="1">
-        <v>0.36990000000000001</v>
+        <v>6.48199265529356E-2</v>
       </c>
       <c r="L36" s="1">
-        <v>0.37480000000000002</v>
+        <v>0.112542641760282</v>
       </c>
       <c r="M36" s="1">
-        <v>11.970599999999999</v>
+        <v>2.6668724105293199E-2</v>
       </c>
       <c r="N36" s="1">
-        <v>0.4118</v>
+        <v>4.7795668440602901E-2</v>
       </c>
       <c r="O36" s="1">
-        <v>0.4118</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P36" s="1">
-        <v>0.34379999999999999</v>
+        <v>6.4820172017016203E-2</v>
       </c>
       <c r="Q36" s="1">
-        <v>0.34320000000000001</v>
+        <v>6.4821297126004901E-2</v>
       </c>
       <c r="R36" s="1">
-        <v>12.769299999999999</v>
+        <v>2.67678718122723E-2</v>
       </c>
       <c r="S36" s="1">
-        <v>8.9023000000000003</v>
+        <v>2.67678718122723E-2</v>
       </c>
       <c r="T36" s="1">
-        <v>8.9023000000000003</v>
+        <v>12.9704648663235</v>
       </c>
       <c r="U36" s="1">
-        <v>8.0999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.74689060519484196</v>
+      </c>
+      <c r="V36" s="1">
+        <v>0.75299751427088202</v>
+      </c>
+      <c r="W36" s="1">
+        <v>3.4374888384884499E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B37">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C37">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D37">
         <v>30</v>
       </c>
       <c r="E37" s="1">
-        <v>11.6381</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F37" s="1">
-        <v>9.6600000000000005E-2</v>
+        <v>2.2577437373898699E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>9.5399999999999999E-2</v>
+        <v>2.2641475112958501E-2</v>
       </c>
       <c r="H37" s="1">
-        <v>11.6431</v>
+        <v>4.8223861228183E-2</v>
       </c>
       <c r="I37" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>4.7380586708574403E-2</v>
       </c>
       <c r="J37" s="1">
-        <v>7.5600000000000001E-2</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K37" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>1.2092997421830899E-2</v>
       </c>
       <c r="L37" s="1">
-        <v>1.52E-2</v>
+        <v>1.7615191951032502E-2</v>
       </c>
       <c r="M37" s="1">
-        <v>13.0025</v>
+        <v>5.0727452754561801E-2</v>
       </c>
       <c r="N37" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>4.5591649403528799E-2</v>
       </c>
       <c r="O37" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P37" s="1">
-        <v>6.3E-3</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="Q37" s="1">
-        <v>6.3E-3</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="R37" s="1">
-        <v>12.6759</v>
+        <v>4.90166757943028E-2</v>
       </c>
       <c r="S37" s="1">
-        <v>0.75719999999999998</v>
+        <v>4.90166757943028E-2</v>
       </c>
       <c r="T37" s="1">
-        <v>0.76480000000000004</v>
+        <v>13.382903227762499</v>
       </c>
       <c r="U37" s="1">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.50512202461532996</v>
+      </c>
+      <c r="V37" s="1">
+        <v>0.54539502650428595</v>
+      </c>
+      <c r="W37" s="1">
+        <v>9.4054337214562895E-6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B38">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C38">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D38">
         <v>35</v>
       </c>
       <c r="E38" s="1">
-        <v>11.6381</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F38" s="1">
-        <v>9.6600000000000005E-2</v>
+        <v>2.2577437373898699E-2</v>
       </c>
       <c r="G38" s="1">
-        <v>9.5399999999999999E-2</v>
+        <v>2.2641475112958501E-2</v>
       </c>
       <c r="H38" s="1">
-        <v>11.6431</v>
+        <v>1.15976068261436E-2</v>
       </c>
       <c r="I38" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>1.14600168233591E-2</v>
       </c>
       <c r="J38" s="1">
-        <v>7.5600000000000001E-2</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K38" s="1">
-        <v>5.0700000000000002E-2</v>
+        <v>1.2092997421830899E-2</v>
       </c>
       <c r="L38" s="1">
-        <v>5.3900000000000003E-2</v>
+        <v>1.7615191951032502E-2</v>
       </c>
       <c r="M38" s="1">
-        <v>13.0025</v>
+        <v>1.09105606668698E-2</v>
       </c>
       <c r="N38" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>1.1984310832698001E-2</v>
       </c>
       <c r="O38" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P38" s="1">
-        <v>3.9300000000000002E-2</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="Q38" s="1">
-        <v>3.9300000000000002E-2</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="R38" s="1">
-        <v>12.4438</v>
+        <v>1.05958588878797E-2</v>
       </c>
       <c r="S38" s="1">
-        <v>0.65649999999999997</v>
+        <v>1.05958588878797E-2</v>
       </c>
       <c r="T38" s="1">
-        <v>0.65620000000000001</v>
+        <v>13.076481423869801</v>
       </c>
       <c r="U38" s="1">
-        <v>1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
+        <v>3.3951311891410298E-2</v>
+      </c>
+      <c r="V38" s="1">
+        <v>3.4532005169517502E-2</v>
+      </c>
+      <c r="W38" s="1">
+        <v>6.1772633905336999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B39">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C39">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D39">
         <v>40</v>
       </c>
       <c r="E39" s="1">
-        <v>11.6381</v>
+        <v>12.337697791618</v>
       </c>
       <c r="F39" s="1">
-        <v>9.6600000000000005E-2</v>
+        <v>2.2577437373898699E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>9.5399999999999999E-2</v>
+        <v>2.2641475112958501E-2</v>
       </c>
       <c r="H39" s="1">
-        <v>11.6431</v>
+        <v>2.1882913511679401E-2</v>
       </c>
       <c r="I39" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>2.21465707371955E-2</v>
       </c>
       <c r="J39" s="1">
-        <v>7.5600000000000001E-2</v>
+        <v>12.345679183253599</v>
       </c>
       <c r="K39" s="1">
-        <v>0.15129999999999999</v>
+        <v>1.2092997421830899E-2</v>
       </c>
       <c r="L39" s="1">
-        <v>0.15409999999999999</v>
+        <v>1.7615191951032502E-2</v>
       </c>
       <c r="M39" s="1">
-        <v>13.0025</v>
+        <v>1.9422603846703301E-2</v>
       </c>
       <c r="N39" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>2.3955673173083801E-2</v>
       </c>
       <c r="O39" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P39" s="1">
-        <v>0.13750000000000001</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="Q39" s="1">
-        <v>0.13750000000000001</v>
+        <v>1.20932363743575E-2</v>
       </c>
       <c r="R39" s="1">
-        <v>12.3033</v>
+        <v>1.9903028787770598E-2</v>
       </c>
       <c r="S39" s="1">
-        <v>0.5222</v>
+        <v>1.9903028787770598E-2</v>
       </c>
       <c r="T39" s="1">
-        <v>0.5222</v>
+        <v>13.0799897718693</v>
       </c>
       <c r="U39" s="1">
-        <v>3.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.3">
+        <v>8.8988527453407698E-2</v>
+      </c>
+      <c r="V39" s="1">
+        <v>8.8988527453407698E-2</v>
+      </c>
+      <c r="W39" s="1">
+        <v>2.9346180977212499E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>5000</v>
       </c>
       <c r="C40">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D40">
         <v>30</v>
       </c>
       <c r="E40" s="1">
-        <v>11.6381</v>
+        <v>11.638114418290399</v>
       </c>
       <c r="F40" s="1">
-        <v>1.35E-2</v>
+        <v>0.75283724616674097</v>
       </c>
       <c r="G40" s="1">
-        <v>1.35E-2</v>
+        <v>0.74902520733601896</v>
       </c>
       <c r="H40" s="1">
-        <v>11.638299999999999</v>
+        <v>6.6191731949107505E-2</v>
       </c>
       <c r="I40" s="1">
-        <v>1.21E-2</v>
+        <v>6.6191731949107505E-2</v>
       </c>
       <c r="J40" s="1">
-        <v>1.2800000000000001E-2</v>
+        <v>11.638270361064301</v>
       </c>
       <c r="K40" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.41113607188918</v>
       </c>
       <c r="L40" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.45026455223869699</v>
       </c>
       <c r="M40" s="1">
-        <v>14.443300000000001</v>
+        <v>4.82993428102007E-2</v>
       </c>
       <c r="N40" s="1">
-        <v>1.21E-2</v>
+        <v>7.6049955949234499E-2</v>
       </c>
       <c r="O40" s="1">
-        <v>1.21E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P40" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.41180448008307702</v>
       </c>
       <c r="Q40" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.41180448008307602</v>
       </c>
       <c r="R40" s="1">
-        <v>12.8733</v>
+        <v>5.0181004992420099E-2</v>
       </c>
       <c r="S40" s="1">
-        <v>0.53139999999999998</v>
+        <v>5.0264046638252E-2</v>
       </c>
       <c r="T40" s="1">
-        <v>0.5353</v>
+        <v>12.5992922731568</v>
       </c>
       <c r="U40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.3">
+        <v>6.4514378940881603</v>
+      </c>
+      <c r="V40" s="1">
+        <v>6.5859240851258001</v>
+      </c>
+      <c r="W40" s="1">
+        <v>4.4934757244565098E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>5000</v>
       </c>
       <c r="C41">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D41">
         <v>35</v>
       </c>
       <c r="E41" s="1">
-        <v>11.6381</v>
+        <v>11.638114418290399</v>
       </c>
       <c r="F41" s="1">
-        <v>1.35E-2</v>
+        <v>0.75283724616674097</v>
       </c>
       <c r="G41" s="1">
-        <v>1.35E-2</v>
+        <v>0.74902520733601896</v>
       </c>
       <c r="H41" s="1">
-        <v>11.638299999999999</v>
+        <v>0.10239470457802401</v>
       </c>
       <c r="I41" s="1">
-        <v>1.21E-2</v>
+        <v>0.10239470457802401</v>
       </c>
       <c r="J41" s="1">
-        <v>1.2800000000000001E-2</v>
+        <v>11.638270361064301</v>
       </c>
       <c r="K41" s="1">
-        <v>2.3800000000000002E-2</v>
+        <v>0.41113607188918</v>
       </c>
       <c r="L41" s="1">
-        <v>2.4799999999999999E-2</v>
+        <v>0.45026455223869699</v>
       </c>
       <c r="M41" s="1">
-        <v>14.443300000000001</v>
+        <v>8.0502586919473901E-2</v>
       </c>
       <c r="N41" s="1">
-        <v>1.21E-2</v>
+        <v>0.11638883826978901</v>
       </c>
       <c r="O41" s="1">
-        <v>1.21E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P41" s="1">
-        <v>2.1600000000000001E-2</v>
+        <v>0.41180448008307702</v>
       </c>
       <c r="Q41" s="1">
-        <v>2.1600000000000001E-2</v>
+        <v>0.41180448008307602</v>
       </c>
       <c r="R41" s="1">
-        <v>12.5258</v>
+        <v>8.7918553949188794E-2</v>
       </c>
       <c r="S41" s="1">
-        <v>9.0999999999999998E-2</v>
+        <v>8.7776196842048501E-2</v>
       </c>
       <c r="T41" s="1">
-        <v>9.64E-2</v>
+        <v>12.8043657968239</v>
       </c>
       <c r="U41" s="1">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
+        <v>8.9798634122557495</v>
+      </c>
+      <c r="V41" s="1">
+        <v>9.0038337538431197</v>
+      </c>
+      <c r="W41" s="1">
+        <v>6.5425518732387597E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>5000</v>
       </c>
       <c r="C42">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>40</v>
       </c>
       <c r="E42" s="1">
-        <v>11.6381</v>
+        <v>11.638114418290399</v>
       </c>
       <c r="F42" s="1">
-        <v>1.35E-2</v>
+        <v>0.75283724616674097</v>
       </c>
       <c r="G42" s="1">
-        <v>1.35E-2</v>
+        <v>0.74902520733601896</v>
       </c>
       <c r="H42" s="1">
-        <v>11.638299999999999</v>
+        <v>0.15080904216372601</v>
       </c>
       <c r="I42" s="1">
-        <v>1.21E-2</v>
+        <v>0.15080904216372601</v>
       </c>
       <c r="J42" s="1">
-        <v>1.2800000000000001E-2</v>
+        <v>11.638270361064301</v>
       </c>
       <c r="K42" s="1">
-        <v>0.1193</v>
+        <v>0.41113607188918</v>
       </c>
       <c r="L42" s="1">
-        <v>0.1202</v>
+        <v>0.45026455223869699</v>
       </c>
       <c r="M42" s="1">
-        <v>14.443300000000001</v>
+        <v>0.127351205889706</v>
       </c>
       <c r="N42" s="1">
-        <v>1.21E-2</v>
+        <v>0.16669230837917001</v>
       </c>
       <c r="O42" s="1">
-        <v>1.21E-2</v>
+        <v>14.443349950022901</v>
       </c>
       <c r="P42" s="1">
-        <v>0.1203</v>
+        <v>0.41180448008307702</v>
       </c>
       <c r="Q42" s="1">
-        <v>0.1203</v>
+        <v>0.41180448008307602</v>
       </c>
       <c r="R42" s="1">
-        <v>12.4252</v>
+        <v>0.137648470426459</v>
       </c>
       <c r="S42" s="1">
-        <v>1.24E-2</v>
+        <v>0.13738377518037001</v>
       </c>
       <c r="T42" s="1">
-        <v>1.24E-2</v>
+        <v>12.7693341771758</v>
       </c>
       <c r="U42" s="1">
-        <v>2.8999999999999998E-3</v>
+        <v>8.90234868698826</v>
+      </c>
+      <c r="V42" s="1">
+        <v>8.9023486869882493</v>
+      </c>
+      <c r="W42" s="1">
+        <v>8.1341412779484205E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>5000</v>
+      </c>
+      <c r="C43">
+        <v>20</v>
+      </c>
+      <c r="D43">
+        <v>30</v>
+      </c>
+      <c r="E43" s="1">
+        <v>11.638114418290399</v>
+      </c>
+      <c r="F43" s="1">
+        <v>9.6632557501139194E-2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>9.5428718064289902E-2</v>
+      </c>
+      <c r="H43" s="1">
+        <v>3.8138656729448897E-2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>3.8721456294497199E-2</v>
+      </c>
+      <c r="J43" s="1">
+        <v>11.638270361064301</v>
+      </c>
+      <c r="K43" s="1">
+        <v>6.4819926565504102E-2</v>
+      </c>
+      <c r="L43" s="1">
+        <v>7.5628117596320502E-2</v>
+      </c>
+      <c r="M43" s="1">
+        <v>4.4681901881880502E-2</v>
+      </c>
+      <c r="N43" s="1">
+        <v>3.7436999468215999E-2</v>
+      </c>
+      <c r="O43" s="1">
+        <v>14.443349950022901</v>
+      </c>
+      <c r="P43" s="1">
+        <v>6.4820031104271203E-2</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>6.4820031104271203E-2</v>
+      </c>
+      <c r="R43" s="1">
+        <v>4.2848437586811797E-2</v>
+      </c>
+      <c r="S43" s="1">
+        <v>4.2848437586811797E-2</v>
+      </c>
+      <c r="T43" s="1">
+        <v>12.675920938694</v>
+      </c>
+      <c r="U43" s="1">
+        <v>0.75723705309782097</v>
+      </c>
+      <c r="V43" s="1">
+        <v>0.76482630455692202</v>
+      </c>
+      <c r="W43" s="1">
+        <v>2.09697518076688E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>5000</v>
+      </c>
+      <c r="C44">
+        <v>20</v>
+      </c>
+      <c r="D44">
+        <v>35</v>
+      </c>
+      <c r="E44" s="1">
+        <v>11.638114418290399</v>
+      </c>
+      <c r="F44" s="1">
+        <v>9.6632557501139194E-2</v>
+      </c>
+      <c r="G44" s="1">
+        <v>9.5428718064289902E-2</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1.3890802695819399E-2</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1.4780093621847601E-2</v>
+      </c>
+      <c r="J44" s="1">
+        <v>11.638270361064301</v>
+      </c>
+      <c r="K44" s="1">
+        <v>6.4819926565504102E-2</v>
+      </c>
+      <c r="L44" s="1">
+        <v>7.5628117596320502E-2</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1.34219062294537E-2</v>
+      </c>
+      <c r="N44" s="1">
+        <v>1.46813693689491E-2</v>
+      </c>
+      <c r="O44" s="1">
+        <v>14.443349950022901</v>
+      </c>
+      <c r="P44" s="1">
+        <v>6.4820031104271203E-2</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>6.4820031104271203E-2</v>
+      </c>
+      <c r="R44" s="1">
+        <v>1.24597383778142E-2</v>
+      </c>
+      <c r="S44" s="1">
+        <v>1.24597383778142E-2</v>
+      </c>
+      <c r="T44" s="1">
+        <v>12.443841195865501</v>
+      </c>
+      <c r="U44" s="1">
+        <v>0.65649817841145996</v>
+      </c>
+      <c r="V44" s="1">
+        <v>0.65617076189988999</v>
+      </c>
+      <c r="W44" s="1">
+        <v>1.1223104857344E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>5000</v>
+      </c>
+      <c r="C45">
+        <v>20</v>
+      </c>
+      <c r="D45">
+        <v>40</v>
+      </c>
+      <c r="E45" s="1">
+        <v>11.638114418290399</v>
+      </c>
+      <c r="F45" s="1">
+        <v>9.6632557501139194E-2</v>
+      </c>
+      <c r="G45" s="1">
+        <v>9.5428718064289902E-2</v>
+      </c>
+      <c r="H45" s="1">
+        <v>3.1067297217658399E-2</v>
+      </c>
+      <c r="I45" s="1">
+        <v>3.2101199192799502E-2</v>
+      </c>
+      <c r="J45" s="1">
+        <v>11.638270361064301</v>
+      </c>
+      <c r="K45" s="1">
+        <v>6.4819926565504102E-2</v>
+      </c>
+      <c r="L45" s="1">
+        <v>7.5628117596320502E-2</v>
+      </c>
+      <c r="M45" s="1">
+        <v>2.6668724105293199E-2</v>
+      </c>
+      <c r="N45" s="1">
+        <v>3.2672534645331798E-2</v>
+      </c>
+      <c r="O45" s="1">
+        <v>14.443349950022901</v>
+      </c>
+      <c r="P45" s="1">
+        <v>6.4820031104271203E-2</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>6.4820031104271203E-2</v>
+      </c>
+      <c r="R45" s="1">
+        <v>2.6226728248446299E-2</v>
+      </c>
+      <c r="S45" s="1">
+        <v>2.6226728248446299E-2</v>
+      </c>
+      <c r="T45" s="1">
+        <v>12.303310483265699</v>
+      </c>
+      <c r="U45" s="1">
+        <v>0.52221473616484704</v>
+      </c>
+      <c r="V45" s="1">
+        <v>0.52221473616484704</v>
+      </c>
+      <c r="W45" s="1">
+        <v>3.4374888384884499E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>5000</v>
+      </c>
+      <c r="C46">
+        <v>25</v>
+      </c>
+      <c r="D46">
+        <v>30</v>
+      </c>
+      <c r="E46" s="1">
+        <v>11.638114418290399</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1.3484599565865301E-2</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1.34954707837642E-2</v>
+      </c>
+      <c r="H46" s="1">
+        <v>5.0295279027867103E-2</v>
+      </c>
+      <c r="I46" s="1">
+        <v>5.0295279027867103E-2</v>
+      </c>
+      <c r="J46" s="1">
+        <v>11.638270361064301</v>
+      </c>
+      <c r="K46" s="1">
+        <v>1.20929970936073E-2</v>
+      </c>
+      <c r="L46" s="1">
+        <v>1.28304991516206E-2</v>
+      </c>
+      <c r="M46" s="1">
+        <v>5.0727452754561801E-2</v>
+      </c>
+      <c r="N46" s="1">
+        <v>5.0183842496686303E-2</v>
+      </c>
+      <c r="O46" s="1">
+        <v>14.443349950022901</v>
+      </c>
+      <c r="P46" s="1">
+        <v>1.20932363743575E-2</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>1.20932363743575E-2</v>
+      </c>
+      <c r="R46" s="1">
+        <v>4.90166757943028E-2</v>
+      </c>
+      <c r="S46" s="1">
+        <v>4.90166757943028E-2</v>
+      </c>
+      <c r="T46" s="1">
+        <v>12.8733200672573</v>
+      </c>
+      <c r="U46" s="1">
+        <v>0.53135886856311898</v>
+      </c>
+      <c r="V46" s="1">
+        <v>0.53526527729046103</v>
+      </c>
+      <c r="W46" s="1">
+        <v>9.4054337214562895E-6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>5000</v>
+      </c>
+      <c r="C47">
+        <v>25</v>
+      </c>
+      <c r="D47">
+        <v>35</v>
+      </c>
+      <c r="E47" s="1">
+        <v>11.638114418290399</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1.3484599565865301E-2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1.34954707837642E-2</v>
+      </c>
+      <c r="H47" s="1">
+        <v>1.1228076057910799E-2</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1.1228076057910799E-2</v>
+      </c>
+      <c r="J47" s="1">
+        <v>11.638270361064301</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1.20929970936073E-2</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1.28304991516206E-2</v>
+      </c>
+      <c r="M47" s="1">
+        <v>1.09105606668698E-2</v>
+      </c>
+      <c r="N47" s="1">
+        <v>1.14191101113636E-2</v>
+      </c>
+      <c r="O47" s="1">
+        <v>14.443349950022901</v>
+      </c>
+      <c r="P47" s="1">
+        <v>1.20932363743575E-2</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>1.20932363743575E-2</v>
+      </c>
+      <c r="R47" s="1">
+        <v>1.05958588878797E-2</v>
+      </c>
+      <c r="S47" s="1">
+        <v>1.05958588878797E-2</v>
+      </c>
+      <c r="T47" s="1">
+        <v>12.5258034717324</v>
+      </c>
+      <c r="U47" s="1">
+        <v>9.0990018618450005E-2</v>
+      </c>
+      <c r="V47" s="1">
+        <v>9.6401271055544996E-2</v>
+      </c>
+      <c r="W47" s="1">
+        <v>6.1772633905336999E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>5000</v>
+      </c>
+      <c r="C48">
+        <v>25</v>
+      </c>
+      <c r="D48">
+        <v>40</v>
+      </c>
+      <c r="E48" s="1">
+        <v>11.638114418290399</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1.3484599565865301E-2</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1.34954707837642E-2</v>
+      </c>
+      <c r="H48" s="1">
+        <v>2.01518970105008E-2</v>
+      </c>
+      <c r="I48" s="1">
+        <v>2.01518970105008E-2</v>
+      </c>
+      <c r="J48" s="1">
+        <v>11.638270361064301</v>
+      </c>
+      <c r="K48" s="1">
+        <v>1.20929970936073E-2</v>
+      </c>
+      <c r="L48" s="1">
+        <v>1.28304991516206E-2</v>
+      </c>
+      <c r="M48" s="1">
+        <v>1.9422603846703301E-2</v>
+      </c>
+      <c r="N48" s="1">
+        <v>2.0507100953639501E-2</v>
+      </c>
+      <c r="O48" s="1">
+        <v>14.443349950022901</v>
+      </c>
+      <c r="P48" s="1">
+        <v>1.20932363743575E-2</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>1.20932363743575E-2</v>
+      </c>
+      <c r="R48" s="1">
+        <v>1.9903028787770598E-2</v>
+      </c>
+      <c r="S48" s="1">
+        <v>1.9903028787770598E-2</v>
+      </c>
+      <c r="T48" s="1">
+        <v>12.4252189812963</v>
+      </c>
+      <c r="U48" s="1">
+        <v>1.2423745933668099E-2</v>
+      </c>
+      <c r="V48" s="1">
+        <v>1.2423745933668099E-2</v>
+      </c>
+      <c r="W48" s="1">
+        <v>2.9346180977212499E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
figures and values square
</commit_message>
<xml_diff>
--- a/Objective values.xlsx
+++ b/Objective values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/sabetancurgi_unal_edu_co/Documents/Escritorio/S and C/accessibility-iamod_njp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{9CA4AC84-12D3-4F0D-81C3-B70202E6BC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D24B416-50F8-4BC6-9A8B-647E09066F05}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{9CA4AC84-12D3-4F0D-81C3-B70202E6BC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EFD04B2-BAC0-4191-982A-D1BE871E7A41}"/>
   <bookViews>
-    <workbookView xWindow="6192" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{24270E23-22B1-443F-A580-B5632CFE18BD}"/>
+    <workbookView xWindow="7755" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{24270E23-22B1-443F-A580-B5632CFE18BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,10 +470,10 @@
   <dimension ref="B1:W48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,16 +1296,16 @@
         <v>0.23259518537038401</v>
       </c>
       <c r="T13" s="1">
-        <v>15.6907683421269</v>
+        <v>15.579750353475299</v>
       </c>
       <c r="U13" s="1">
-        <v>19.0062674598034</v>
+        <v>17.021481171950001</v>
       </c>
       <c r="V13" s="1">
-        <v>19.006523481988101</v>
+        <v>17.021607898223198</v>
       </c>
       <c r="W13" s="1">
-        <v>6.02072767102412E-3</v>
+        <v>2.1543857891664201E-3</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
@@ -1364,16 +1364,16 @@
         <v>0.30268255312697301</v>
       </c>
       <c r="T14" s="1">
-        <v>15.6790404756375</v>
+        <v>15.6132855214661</v>
       </c>
       <c r="U14" s="1">
-        <v>19.550378179535301</v>
+        <v>17.900906098794401</v>
       </c>
       <c r="V14" s="1">
-        <v>19.5503914774281</v>
+        <v>17.8994459647305</v>
       </c>
       <c r="W14" s="1">
-        <v>8.2268850107369198E-3</v>
+        <v>3.2601209394831098E-3</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
@@ -1432,16 +1432,16 @@
         <v>0.36389786770483601</v>
       </c>
       <c r="T15" s="1">
-        <v>15.6835984331488</v>
+        <v>15.682967789253899</v>
       </c>
       <c r="U15" s="1">
-        <v>19.503767884735499</v>
+        <v>18.894285164794901</v>
       </c>
       <c r="V15" s="1">
-        <v>19.504550979491398</v>
+        <v>18.8964740265816</v>
       </c>
       <c r="W15" s="1">
-        <v>9.4247245338952707E-3</v>
+        <v>4.1889498838416899E-3</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
@@ -1500,16 +1500,16 @@
         <v>1.37927113841465E-2</v>
       </c>
       <c r="T16" s="1">
-        <v>15.5506810100533</v>
+        <v>15.3373289265569</v>
       </c>
       <c r="U16" s="1">
-        <v>2.5052300847300701</v>
+        <v>1.87038660857343</v>
       </c>
       <c r="V16" s="1">
-        <v>2.6493334201941798</v>
+        <v>1.8630447294889201</v>
       </c>
       <c r="W16" s="1">
-        <v>2.5898675302204099E-4</v>
+        <v>2.1448621537529901E-5</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
@@ -1568,16 +1568,16 @@
         <v>3.9901581891417903E-2</v>
       </c>
       <c r="T17" s="1">
-        <v>15.520865257280599</v>
+        <v>15.3912312075096</v>
       </c>
       <c r="U17" s="1">
-        <v>4.2328599361825896</v>
+        <v>3.39060418704676</v>
       </c>
       <c r="V17" s="1">
-        <v>4.2328599361825896</v>
+        <v>3.3904720877499801</v>
       </c>
       <c r="W17" s="1">
-        <v>1.88560115810021E-3</v>
+        <v>3.2781251260287001E-4</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
@@ -1636,16 +1636,16 @@
         <v>8.4590897117651304E-2</v>
       </c>
       <c r="T18" s="1">
-        <v>15.514396251254899</v>
+        <v>15.4012446651919</v>
       </c>
       <c r="U18" s="1">
-        <v>4.5413212682056896</v>
+        <v>3.6888090138851899</v>
       </c>
       <c r="V18" s="1">
-        <v>4.5430706145075703</v>
+        <v>3.6890717142934499</v>
       </c>
       <c r="W18" s="1">
-        <v>4.3128861882991499E-3</v>
+        <v>9.7116606816001299E-4</v>
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
@@ -1704,16 +1704,16 @@
         <v>2.57765038772611E-2</v>
       </c>
       <c r="T19" s="1">
-        <v>15.492172085366001</v>
+        <v>15.7368213871005</v>
       </c>
       <c r="U19" s="1">
-        <v>1.1793641690380601</v>
+        <v>1.17716779061782</v>
       </c>
       <c r="V19" s="1">
-        <v>1.17584155954029</v>
+        <v>1.17716779061782</v>
       </c>
       <c r="W19" s="1">
-        <v>9.4054337214562895E-6</v>
+        <v>3.1342752169547099E-7</v>
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
@@ -1772,16 +1772,16 @@
         <v>9.2562442506826294E-3</v>
       </c>
       <c r="T20" s="1">
-        <v>15.364969014623099</v>
+        <v>15.334430922831899</v>
       </c>
       <c r="U20" s="1">
-        <v>0.47987204632595798</v>
+        <v>0.59541791989840198</v>
       </c>
       <c r="V20" s="1">
-        <v>0.52240024224002202</v>
+        <v>0.59541407266858204</v>
       </c>
       <c r="W20" s="1">
-        <v>6.5393883819689499E-4</v>
+        <v>6.1327053976945896E-5</v>
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
@@ -1840,16 +1840,16 @@
         <v>3.0924340577898401E-2</v>
       </c>
       <c r="T21" s="1">
-        <v>15.513054290946</v>
+        <v>15.3748806484939</v>
       </c>
       <c r="U21" s="1">
-        <v>0.99416038552628705</v>
+        <v>0.86675747048060103</v>
       </c>
       <c r="V21" s="1">
-        <v>1.0019474124377501</v>
+        <v>0.86691668342397898</v>
       </c>
       <c r="W21" s="1">
-        <v>3.0622499821415699E-3</v>
+        <v>4.6926626837150799E-4</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
@@ -1908,16 +1908,16 @@
         <v>0.141902794644062</v>
       </c>
       <c r="T22" s="1">
-        <v>14.5947445747959</v>
+        <v>14.516634211657401</v>
       </c>
       <c r="U22" s="1">
-        <v>15.574646849745999</v>
+        <v>13.0758831169444</v>
       </c>
       <c r="V22" s="1">
-        <v>15.5748949626495</v>
+        <v>13.076827957316601</v>
       </c>
       <c r="W22" s="1">
-        <v>4.8070695525870904E-3</v>
+        <v>1.61864081803668E-3</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
@@ -1976,16 +1976,16 @@
         <v>0.20624140791397599</v>
       </c>
       <c r="T23" s="1">
-        <v>14.559977366042</v>
+        <v>14.539535515907801</v>
       </c>
       <c r="U23" s="1">
-        <v>16.388541675938502</v>
+        <v>15.245760178260699</v>
       </c>
       <c r="V23" s="1">
-        <v>16.388541675938502</v>
+        <v>15.227502768254899</v>
       </c>
       <c r="W23" s="1">
-        <v>7.0038676231975704E-3</v>
+        <v>2.5803986264241502E-3</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
@@ -2044,16 +2044,16 @@
         <v>0.26723683388099201</v>
       </c>
       <c r="T24" s="1">
-        <v>14.551429352652701</v>
+        <v>14.550231060266899</v>
       </c>
       <c r="U24" s="1">
-        <v>16.382721600328999</v>
+        <v>15.5013665940139</v>
       </c>
       <c r="V24" s="1">
-        <v>16.382772260880099</v>
+        <v>15.468692017594201</v>
       </c>
       <c r="W24" s="1">
-        <v>8.4878830630759298E-3</v>
+        <v>3.4803908842232201E-3</v>
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
@@ -2112,16 +2112,16 @@
         <v>1.89696883110698E-2</v>
       </c>
       <c r="T25" s="1">
-        <v>14.1965967559644</v>
+        <v>13.786223762814</v>
       </c>
       <c r="U25" s="1">
-        <v>1.43796441332221</v>
+        <v>0.66063657160254396</v>
       </c>
       <c r="V25" s="1">
-        <v>1.43992870549402</v>
+        <v>0.68884895646424604</v>
       </c>
       <c r="W25" s="1">
-        <v>2.09697518076688E-4</v>
+        <v>1.6852065228841999E-5</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
@@ -2180,16 +2180,16 @@
         <v>1.7449701217725499E-2</v>
       </c>
       <c r="T26" s="1">
-        <v>14.2919997464018</v>
+        <v>14.0070021225304</v>
       </c>
       <c r="U26" s="1">
-        <v>2.33446481434741</v>
+        <v>1.06678369869075</v>
       </c>
       <c r="V26" s="1">
-        <v>2.2453330552775101</v>
+        <v>1.04325017432579</v>
       </c>
       <c r="W26" s="1">
-        <v>1.15852298487793E-3</v>
+        <v>1.72901989445172E-4</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
@@ -2248,16 +2248,16 @@
         <v>4.7299405314665303E-2</v>
       </c>
       <c r="T27" s="1">
-        <v>14.3449073829388</v>
+        <v>14.1488570309546</v>
       </c>
       <c r="U27" s="1">
-        <v>3.0187565911988199</v>
+        <v>2.1309650170560501</v>
       </c>
       <c r="V27" s="1">
-        <v>3.0202021979013201</v>
+        <v>2.1176026617924699</v>
       </c>
       <c r="W27" s="1">
-        <v>3.5851891206514701E-3</v>
+        <v>6.8231060381754999E-4</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
@@ -2316,16 +2316,16 @@
         <v>4.90166757943028E-2</v>
       </c>
       <c r="T28" s="1">
-        <v>14.266180131436499</v>
+        <v>14.4019086649791</v>
       </c>
       <c r="U28" s="1">
-        <v>0.51353306983106295</v>
+        <v>0.91874436674812898</v>
       </c>
       <c r="V28" s="1">
-        <v>0.601716995400984</v>
+        <v>1.00411458314247</v>
       </c>
       <c r="W28" s="1">
-        <v>9.4054337214562895E-6</v>
+        <v>3.13427521695926E-7</v>
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
@@ -2384,16 +2384,16 @@
         <v>1.05958588878797E-2</v>
       </c>
       <c r="T29" s="1">
-        <v>14.183587898088399</v>
+        <v>13.9437087813871</v>
       </c>
       <c r="U29" s="1">
-        <v>0.13768856848139599</v>
+        <v>0.115517870908374</v>
       </c>
       <c r="V29" s="1">
-        <v>0.13768856848139599</v>
+        <v>0.115517870908374</v>
       </c>
       <c r="W29" s="1">
-        <v>6.1772633905336999E-4</v>
+        <v>5.4178941282424999E-5</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
@@ -2452,16 +2452,16 @@
         <v>1.9903028787770598E-2</v>
       </c>
       <c r="T30" s="1">
-        <v>14.086816463182201</v>
+        <v>13.6603035280811</v>
       </c>
       <c r="U30" s="1">
-        <v>9.5840796137552503E-2</v>
+        <v>2.4444814902255401E-2</v>
       </c>
       <c r="V30" s="1">
-        <v>9.5840796137552503E-2</v>
+        <v>3.03957250212098E-2</v>
       </c>
       <c r="W30" s="1">
-        <v>2.9346180977212499E-3</v>
+        <v>4.2590482568528301E-4</v>
       </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
@@ -2520,16 +2520,16 @@
         <v>8.8391809732441207E-2</v>
       </c>
       <c r="T31" s="1">
-        <v>13.4455091631944</v>
+        <v>13.4154865178308</v>
       </c>
       <c r="U31" s="1">
-        <v>10.6526413833353</v>
+        <v>8.8838905219535906</v>
       </c>
       <c r="V31" s="1">
-        <v>10.6438539044631</v>
+        <v>8.7815108992329005</v>
       </c>
       <c r="W31" s="1">
-        <v>4.4934757244565098E-3</v>
+        <v>1.4996423274823401E-3</v>
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
@@ -2588,16 +2588,16 @@
         <v>0.14298658358979</v>
       </c>
       <c r="T32" s="1">
-        <v>13.507023206513299</v>
+        <v>13.488212088292601</v>
       </c>
       <c r="U32" s="1">
-        <v>11.986642717232399</v>
+        <v>11.6011871992241</v>
       </c>
       <c r="V32" s="1">
-        <v>11.992529156781099</v>
+        <v>11.464277009181099</v>
       </c>
       <c r="W32" s="1">
-        <v>6.5698424523034397E-3</v>
+        <v>2.3055782250070902E-3</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
@@ -2656,16 +2656,16 @@
         <v>0.20047781314736801</v>
       </c>
       <c r="T33" s="1">
-        <v>13.506936703965399</v>
+        <v>13.4493877525701</v>
       </c>
       <c r="U33" s="1">
-        <v>11.9711502929815</v>
+        <v>11.254330159209401</v>
       </c>
       <c r="V33" s="1">
-        <v>11.970911727915301</v>
+        <v>11.1644269742297</v>
       </c>
       <c r="W33" s="1">
-        <v>8.1496446174726695E-3</v>
+        <v>3.1948337357229901E-3</v>
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
@@ -2724,16 +2724,16 @@
         <v>4.2041693454294399E-2</v>
       </c>
       <c r="T34" s="1">
-        <v>13.173204705537501</v>
+        <v>12.7074251381341</v>
       </c>
       <c r="U34" s="1">
-        <v>0.98175480704001195</v>
+        <v>0.223412643173623</v>
       </c>
       <c r="V34" s="1">
-        <v>0.98668828456444402</v>
+        <v>0.26917716361289501</v>
       </c>
       <c r="W34" s="1">
-        <v>2.09697518076688E-4</v>
+        <v>1.6850155423055E-5</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
@@ -2792,16 +2792,16 @@
         <v>1.25167832687758E-2</v>
       </c>
       <c r="T35" s="1">
-        <v>13.024396645161399</v>
+        <v>12.655349256227399</v>
       </c>
       <c r="U35" s="1">
-        <v>0.894494668949945</v>
+        <v>0.181339652993429</v>
       </c>
       <c r="V35" s="1">
-        <v>0.894494668949946</v>
+        <v>0.18362453841707499</v>
       </c>
       <c r="W35" s="1">
-        <v>1.1223104857344E-3</v>
+        <v>1.6539494629814699E-4</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
@@ -2860,16 +2860,16 @@
         <v>2.67678718122723E-2</v>
       </c>
       <c r="T36" s="1">
-        <v>12.9704648663235</v>
+        <v>12.9790954608777</v>
       </c>
       <c r="U36" s="1">
-        <v>0.74689060519484196</v>
+        <v>0.43923130490677698</v>
       </c>
       <c r="V36" s="1">
-        <v>0.75299751427088202</v>
+        <v>0.46084613765128701</v>
       </c>
       <c r="W36" s="1">
-        <v>3.4374888384884499E-3</v>
+        <v>6.19578282181649E-4</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
@@ -2928,16 +2928,16 @@
         <v>4.90166757943028E-2</v>
       </c>
       <c r="T37" s="1">
-        <v>13.382903227762499</v>
+        <v>13.257740588890201</v>
       </c>
       <c r="U37" s="1">
-        <v>0.50512202461532996</v>
+        <v>0.46546668697346799</v>
       </c>
       <c r="V37" s="1">
-        <v>0.54539502650428595</v>
+        <v>0.46664741860531</v>
       </c>
       <c r="W37" s="1">
-        <v>9.4054337214562895E-6</v>
+        <v>3.1364705384216898E-7</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
@@ -2996,16 +2996,16 @@
         <v>1.05958588878797E-2</v>
       </c>
       <c r="T38" s="1">
-        <v>13.076481423869801</v>
+        <v>12.454552110318801</v>
       </c>
       <c r="U38" s="1">
-        <v>3.3951311891410298E-2</v>
+        <v>1.2684090681526801E-2</v>
       </c>
       <c r="V38" s="1">
-        <v>3.4532005169517502E-2</v>
+        <v>1.25866161755198E-2</v>
       </c>
       <c r="W38" s="1">
-        <v>6.1772633905336999E-4</v>
+        <v>5.4463020771851297E-5</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
@@ -3064,16 +3064,16 @@
         <v>1.9903028787770598E-2</v>
       </c>
       <c r="T39" s="1">
-        <v>13.0799897718693</v>
+        <v>12.4923832433483</v>
       </c>
       <c r="U39" s="1">
-        <v>8.8988527453407698E-2</v>
+        <v>1.3474105329702999E-2</v>
       </c>
       <c r="V39" s="1">
-        <v>8.8988527453407698E-2</v>
+        <v>1.2552358726014101E-2</v>
       </c>
       <c r="W39" s="1">
-        <v>2.9346180977212499E-3</v>
+        <v>4.2591225612303302E-4</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
@@ -3132,16 +3132,16 @@
         <v>5.0264046638252E-2</v>
       </c>
       <c r="T40" s="1">
-        <v>12.5992922731568</v>
+        <v>11.910637107833301</v>
       </c>
       <c r="U40" s="1">
-        <v>6.4514378940881603</v>
+        <v>1.29224480095224</v>
       </c>
       <c r="V40" s="1">
-        <v>6.5859240851258001</v>
+        <v>1.2324058648476</v>
       </c>
       <c r="W40" s="1">
-        <v>4.4934757244565098E-3</v>
+        <v>1.4996667658895501E-3</v>
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
@@ -3200,16 +3200,16 @@
         <v>8.7776196842048501E-2</v>
       </c>
       <c r="T41" s="1">
-        <v>12.8043657968239</v>
+        <v>11.957051337013301</v>
       </c>
       <c r="U41" s="1">
-        <v>8.9798634122557495</v>
+        <v>1.57724608827539</v>
       </c>
       <c r="V41" s="1">
-        <v>9.0038337538431197</v>
+        <v>1.6122134527930001</v>
       </c>
       <c r="W41" s="1">
-        <v>6.5425518732387597E-3</v>
+        <v>2.3000794293604201E-3</v>
       </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
@@ -3268,16 +3268,16 @@
         <v>0.13738377518037001</v>
       </c>
       <c r="T42" s="1">
-        <v>12.7693341771758</v>
+        <v>11.919627832740201</v>
       </c>
       <c r="U42" s="1">
-        <v>8.90234868698826</v>
+        <v>1.5161627818275401</v>
       </c>
       <c r="V42" s="1">
-        <v>8.9023486869882493</v>
+        <v>1.5089374337874899</v>
       </c>
       <c r="W42" s="1">
-        <v>8.1341412779484205E-3</v>
+        <v>3.1837894900912799E-3</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
@@ -3336,16 +3336,16 @@
         <v>4.2848437586811797E-2</v>
       </c>
       <c r="T43" s="1">
-        <v>12.675920938694</v>
+        <v>11.763716808226199</v>
       </c>
       <c r="U43" s="1">
-        <v>0.75723705309782097</v>
+        <v>8.7305542854317103E-2</v>
       </c>
       <c r="V43" s="1">
-        <v>0.76482630455692202</v>
+        <v>9.1078086438149602E-2</v>
       </c>
       <c r="W43" s="1">
-        <v>2.09697518076688E-4</v>
+        <v>1.6849893719218501E-5</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
@@ -3404,16 +3404,16 @@
         <v>1.24597383778142E-2</v>
       </c>
       <c r="T44" s="1">
-        <v>12.443841195865501</v>
+        <v>11.749854916832</v>
       </c>
       <c r="U44" s="1">
-        <v>0.65649817841145996</v>
+        <v>8.2241369587612204E-2</v>
       </c>
       <c r="V44" s="1">
-        <v>0.65617076189988999</v>
+        <v>7.9585171189683196E-2</v>
       </c>
       <c r="W44" s="1">
-        <v>1.1223104857344E-3</v>
+        <v>1.64344451552019E-4</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
@@ -3472,16 +3472,16 @@
         <v>2.6226728248446299E-2</v>
       </c>
       <c r="T45" s="1">
-        <v>12.303310483265699</v>
+        <v>11.782094577052201</v>
       </c>
       <c r="U45" s="1">
-        <v>0.52221473616484704</v>
+        <v>9.3722710975636905E-2</v>
       </c>
       <c r="V45" s="1">
-        <v>0.52221473616484704</v>
+        <v>9.4752640655732398E-2</v>
       </c>
       <c r="W45" s="1">
-        <v>3.4374888384884499E-3</v>
+        <v>6.1958095290298297E-4</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
@@ -3540,16 +3540,16 @@
         <v>4.90166757943028E-2</v>
       </c>
       <c r="T46" s="1">
-        <v>12.8733200672573</v>
+        <v>12.977945701256299</v>
       </c>
       <c r="U46" s="1">
-        <v>0.53135886856311898</v>
+        <v>0.99823784259652104</v>
       </c>
       <c r="V46" s="1">
-        <v>0.53526527729046103</v>
+        <v>0.99823784259652104</v>
       </c>
       <c r="W46" s="1">
-        <v>9.4054337214562895E-6</v>
+        <v>3.1342752169547099E-7</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
@@ -3608,16 +3608,16 @@
         <v>1.05958588878797E-2</v>
       </c>
       <c r="T47" s="1">
-        <v>12.5258034717324</v>
+        <v>12.4393573218436</v>
       </c>
       <c r="U47" s="1">
-        <v>9.0990018618450005E-2</v>
+        <v>3.22329954563546E-2</v>
       </c>
       <c r="V47" s="1">
-        <v>9.6401271055544996E-2</v>
+        <v>3.3050250417763299E-2</v>
       </c>
       <c r="W47" s="1">
-        <v>6.1772633905336999E-4</v>
+        <v>5.4195746531310103E-5</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
@@ -3676,16 +3676,16 @@
         <v>1.9903028787770598E-2</v>
       </c>
       <c r="T48" s="1">
-        <v>12.4252189812963</v>
+        <v>11.77435193354</v>
       </c>
       <c r="U48" s="1">
-        <v>1.2423745933668099E-2</v>
+        <v>1.38253393984578E-2</v>
       </c>
       <c r="V48" s="1">
-        <v>1.2423745933668099E-2</v>
+        <v>1.26810514797586E-2</v>
       </c>
       <c r="W48" s="1">
-        <v>2.9346180977212499E-3</v>
+        <v>4.2590077871337199E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>